<commit_message>
added more data over the weekend
</commit_message>
<xml_diff>
--- a/data/exp_raw/no2_analyticall_results.xlsx
+++ b/data/exp_raw/no2_analyticall_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vcantarella/Documents/FuhrbergerColumns/data/exp_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7075DD9-FD24-5745-945B-D02AF71AFF03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58CAF937-47F7-2343-BAC0-CA7AD2A077D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="740" windowWidth="28040" windowHeight="16680" activeTab="5" xr2:uid="{3CD87C21-EA08-D841-BE93-D5199CA9A403}"/>
   </bookViews>
@@ -7960,10 +7960,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28553D95-A703-174C-8A27-2C251D35502B}">
-  <dimension ref="A1:N217"/>
+  <dimension ref="A1:N241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A132" zoomScale="110" workbookViewId="0">
-      <selection activeCell="I142" sqref="I142:J145"/>
+    <sheetView tabSelected="1" topLeftCell="A201" zoomScale="110" workbookViewId="0">
+      <selection activeCell="I210" sqref="I210:I213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13895,15 +13895,15 @@
         <v>45799.730555555558</v>
       </c>
       <c r="E194" s="1">
-        <v>45799.416666666664</v>
+        <v>45800.416666666664</v>
       </c>
       <c r="F194" s="1">
         <f t="shared" si="9"/>
-        <v>45799.573611111111</v>
+        <v>45800.073611111111</v>
       </c>
       <c r="G194">
-        <f t="shared" ref="G194:G201" si="10" xml:space="preserve"> F194-IF(OR(B194=1,B194=2),$M$2,$M$3)</f>
-        <v>9.7402777777751908</v>
+        <f t="shared" ref="G194:G229" si="10" xml:space="preserve"> F194-IF(OR(B194=1,B194=2),$M$2,$M$3)</f>
+        <v>10.240277777775191</v>
       </c>
       <c r="H194">
         <v>30.6</v>
@@ -13921,22 +13921,22 @@
         <v>2</v>
       </c>
       <c r="C195" t="str">
-        <f t="shared" ref="C195:C217" si="11">_xlfn.CONCAT("F",B195,"-",A195)</f>
+        <f t="shared" ref="C195:C241" si="11">_xlfn.CONCAT("F",B195,"-",A195)</f>
         <v>F2-49</v>
       </c>
       <c r="D195" s="1">
         <v>45799.730555555558</v>
       </c>
       <c r="E195" s="1">
-        <v>45799.416666666664</v>
+        <v>45800.416666666664</v>
       </c>
       <c r="F195" s="1">
-        <f t="shared" ref="F195:F201" si="12">(E195-D195)/2+D195</f>
-        <v>45799.573611111111</v>
+        <f t="shared" ref="F195:F229" si="12">(E195-D195)/2+D195</f>
+        <v>45800.073611111111</v>
       </c>
       <c r="G195">
         <f t="shared" si="10"/>
-        <v>9.7402777777751908</v>
+        <v>10.240277777775191</v>
       </c>
       <c r="H195">
         <v>32.299999999999997</v>
@@ -13961,15 +13961,15 @@
         <v>45799.730555555558</v>
       </c>
       <c r="E196" s="1">
-        <v>45799.416666666664</v>
+        <v>45800.416666666664</v>
       </c>
       <c r="F196" s="1">
         <f t="shared" si="12"/>
-        <v>45799.573611111111</v>
+        <v>45800.073611111111</v>
       </c>
       <c r="G196">
         <f t="shared" si="10"/>
-        <v>9.7305555555576575</v>
+        <v>10.230555555557657</v>
       </c>
       <c r="H196">
         <v>32.44</v>
@@ -13994,15 +13994,15 @@
         <v>45799.730555555558</v>
       </c>
       <c r="E197" s="1">
-        <v>45799.416666666664</v>
+        <v>45800.416666666664</v>
       </c>
       <c r="F197" s="1">
         <f t="shared" si="12"/>
-        <v>45799.573611111111</v>
+        <v>45800.073611111111</v>
       </c>
       <c r="G197">
         <f t="shared" si="10"/>
-        <v>9.7305555555576575</v>
+        <v>10.230555555557657</v>
       </c>
       <c r="H197">
         <v>31.3</v>
@@ -14024,18 +14024,18 @@
         <v>F1-50</v>
       </c>
       <c r="D198" s="1">
-        <v>45799.488888888889</v>
+        <v>45800.488888888889</v>
       </c>
       <c r="E198" s="1">
-        <v>45799.56527777778</v>
+        <v>45800.56527777778</v>
       </c>
       <c r="F198" s="1">
         <f t="shared" si="12"/>
-        <v>45799.527083333334</v>
+        <v>45800.527083333334</v>
       </c>
       <c r="G198">
         <f t="shared" si="10"/>
-        <v>9.6937499999985448</v>
+        <v>10.693749999998545</v>
       </c>
       <c r="L198">
         <f>VLOOKUP(sampling!C198,fe_plate_1!$C$2:$G$80,5,FALSE)</f>
@@ -14054,18 +14054,18 @@
         <v>F2-50</v>
       </c>
       <c r="D199" s="1">
-        <v>45799.488888888889</v>
+        <v>45800.488888888889</v>
       </c>
       <c r="E199" s="1">
-        <v>45799.56527777778</v>
+        <v>45800.56527777778</v>
       </c>
       <c r="F199" s="1">
         <f t="shared" si="12"/>
-        <v>45799.527083333334</v>
+        <v>45800.527083333334</v>
       </c>
       <c r="G199">
         <f t="shared" si="10"/>
-        <v>9.6937499999985448</v>
+        <v>10.693749999998545</v>
       </c>
       <c r="L199">
         <f>VLOOKUP(sampling!C199,fe_plate_1!$C$2:$G$80,5,FALSE)</f>
@@ -14084,18 +14084,18 @@
         <v>F3-50</v>
       </c>
       <c r="D200" s="1">
-        <v>45799.488888888889</v>
+        <v>45800.488888888889</v>
       </c>
       <c r="E200" s="1">
-        <v>45799.56527777778</v>
+        <v>45800.56527777778</v>
       </c>
       <c r="F200" s="1">
         <f t="shared" si="12"/>
-        <v>45799.527083333334</v>
+        <v>45800.527083333334</v>
       </c>
       <c r="G200">
         <f t="shared" si="10"/>
-        <v>9.6840277777810115</v>
+        <v>10.684027777781012</v>
       </c>
       <c r="L200">
         <f>VLOOKUP(sampling!C200,fe_plate_1!$C$2:$G$80,5,FALSE)</f>
@@ -14114,18 +14114,18 @@
         <v>F4-50</v>
       </c>
       <c r="D201" s="1">
-        <v>45799.488888888889</v>
+        <v>45800.488888888889</v>
       </c>
       <c r="E201" s="1">
-        <v>45799.56527777778</v>
+        <v>45800.56527777778</v>
       </c>
       <c r="F201" s="1">
         <f t="shared" si="12"/>
-        <v>45799.527083333334</v>
+        <v>45800.527083333334</v>
       </c>
       <c r="G201">
         <f t="shared" si="10"/>
-        <v>9.6840277777810115</v>
+        <v>10.684027777781012</v>
       </c>
       <c r="L201">
         <f>VLOOKUP(sampling!C201,fe_plate_1!$C$2:$G$80,5,FALSE)</f>
@@ -14143,7 +14143,29 @@
         <f t="shared" si="11"/>
         <v>F1-51</v>
       </c>
-      <c r="F202" s="1"/>
+      <c r="D202" s="1">
+        <v>45800.568055555559</v>
+      </c>
+      <c r="E202" s="3">
+        <v>45800.714583333334</v>
+      </c>
+      <c r="F202" s="1">
+        <f t="shared" si="12"/>
+        <v>45800.641319444447</v>
+      </c>
+      <c r="G202">
+        <f t="shared" si="10"/>
+        <v>10.807986111110949</v>
+      </c>
+      <c r="H202">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="I202">
+        <v>7.52</v>
+      </c>
+      <c r="J202">
+        <v>1042</v>
+      </c>
     </row>
     <row r="203" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A203">
@@ -14156,7 +14178,29 @@
         <f t="shared" si="11"/>
         <v>F2-51</v>
       </c>
-      <c r="F203" s="1"/>
+      <c r="D203" s="1">
+        <v>45800.568055555559</v>
+      </c>
+      <c r="E203" s="3">
+        <v>45800.714583333334</v>
+      </c>
+      <c r="F203" s="1">
+        <f t="shared" si="12"/>
+        <v>45800.641319444447</v>
+      </c>
+      <c r="G203">
+        <f t="shared" si="10"/>
+        <v>10.807986111110949</v>
+      </c>
+      <c r="H203">
+        <v>34.5</v>
+      </c>
+      <c r="I203">
+        <v>7.56</v>
+      </c>
+      <c r="J203">
+        <v>800</v>
+      </c>
     </row>
     <row r="204" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A204">
@@ -14169,7 +14213,29 @@
         <f t="shared" si="11"/>
         <v>F3-51</v>
       </c>
-      <c r="F204" s="1"/>
+      <c r="D204" s="1">
+        <v>45800.568055555559</v>
+      </c>
+      <c r="E204" s="3">
+        <v>45800.714583333334</v>
+      </c>
+      <c r="F204" s="1">
+        <f t="shared" si="12"/>
+        <v>45800.641319444447</v>
+      </c>
+      <c r="G204">
+        <f t="shared" si="10"/>
+        <v>10.798263888893416</v>
+      </c>
+      <c r="H204">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="I204">
+        <v>7.3</v>
+      </c>
+      <c r="J204">
+        <v>1048</v>
+      </c>
     </row>
     <row r="205" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A205">
@@ -14182,7 +14248,29 @@
         <f t="shared" si="11"/>
         <v>F4-51</v>
       </c>
-      <c r="F205" s="1"/>
+      <c r="D205" s="1">
+        <v>45800.568055555559</v>
+      </c>
+      <c r="E205" s="3">
+        <v>45800.714583333334</v>
+      </c>
+      <c r="F205" s="1">
+        <f t="shared" si="12"/>
+        <v>45800.641319444447</v>
+      </c>
+      <c r="G205">
+        <f t="shared" si="10"/>
+        <v>10.798263888893416</v>
+      </c>
+      <c r="H205">
+        <v>35.1</v>
+      </c>
+      <c r="I205">
+        <v>7.43</v>
+      </c>
+      <c r="J205">
+        <v>941</v>
+      </c>
     </row>
     <row r="206" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A206">
@@ -14195,7 +14283,26 @@
         <f t="shared" si="11"/>
         <v>F1-52</v>
       </c>
-      <c r="F206" s="1"/>
+      <c r="D206" s="3">
+        <v>45800.795138888891</v>
+      </c>
+      <c r="E206" s="1">
+        <v>45801.342361111114</v>
+      </c>
+      <c r="F206" s="1">
+        <f t="shared" si="12"/>
+        <v>45801.068750000006</v>
+      </c>
+      <c r="G206">
+        <f t="shared" si="10"/>
+        <v>11.235416666670062</v>
+      </c>
+      <c r="H206">
+        <v>33.1</v>
+      </c>
+      <c r="J206">
+        <v>1029</v>
+      </c>
     </row>
     <row r="207" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A207">
@@ -14208,7 +14315,29 @@
         <f t="shared" si="11"/>
         <v>F2-52</v>
       </c>
-      <c r="F207" s="1"/>
+      <c r="D207" s="3">
+        <v>45800.795138888891</v>
+      </c>
+      <c r="E207" s="1">
+        <v>45801.342361111114</v>
+      </c>
+      <c r="F207" s="1">
+        <f t="shared" si="12"/>
+        <v>45801.068750000006</v>
+      </c>
+      <c r="G207">
+        <f t="shared" si="10"/>
+        <v>11.235416666670062</v>
+      </c>
+      <c r="H207">
+        <v>34.9</v>
+      </c>
+      <c r="I207">
+        <v>7.66</v>
+      </c>
+      <c r="J207">
+        <v>964</v>
+      </c>
     </row>
     <row r="208" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A208">
@@ -14221,9 +14350,28 @@
         <f t="shared" si="11"/>
         <v>F3-52</v>
       </c>
-      <c r="F208" s="1"/>
-    </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D208" s="3">
+        <v>45800.795138888891</v>
+      </c>
+      <c r="E208" s="1">
+        <v>45801.342361111114</v>
+      </c>
+      <c r="F208" s="1">
+        <f t="shared" si="12"/>
+        <v>45801.068750000006</v>
+      </c>
+      <c r="G208">
+        <f t="shared" si="10"/>
+        <v>11.225694444452529</v>
+      </c>
+      <c r="H208">
+        <v>34.700000000000003</v>
+      </c>
+      <c r="J208">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="209" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A209">
         <v>52</v>
       </c>
@@ -14234,9 +14382,28 @@
         <f t="shared" si="11"/>
         <v>F4-52</v>
       </c>
-      <c r="F209" s="1"/>
-    </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D209" s="3">
+        <v>45800.795138888891</v>
+      </c>
+      <c r="E209" s="1">
+        <v>45801.342361111114</v>
+      </c>
+      <c r="F209" s="1">
+        <f t="shared" si="12"/>
+        <v>45801.068750000006</v>
+      </c>
+      <c r="G209">
+        <f t="shared" si="10"/>
+        <v>11.225694444452529</v>
+      </c>
+      <c r="H209">
+        <v>34.9</v>
+      </c>
+      <c r="J209">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="210" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A210">
         <v>53</v>
       </c>
@@ -14247,9 +14414,28 @@
         <f t="shared" si="11"/>
         <v>F1-53</v>
       </c>
-      <c r="F210" s="1"/>
-    </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D210" s="1">
+        <v>45801.345138888886</v>
+      </c>
+      <c r="E210" s="1">
+        <v>45801.53125</v>
+      </c>
+      <c r="F210" s="1">
+        <f t="shared" si="12"/>
+        <v>45801.438194444447</v>
+      </c>
+      <c r="G210">
+        <f t="shared" si="10"/>
+        <v>11.604861111110949</v>
+      </c>
+      <c r="I210">
+        <v>7.62</v>
+      </c>
+      <c r="J210">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="211" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A211">
         <v>53</v>
       </c>
@@ -14260,9 +14446,28 @@
         <f t="shared" si="11"/>
         <v>F2-53</v>
       </c>
-      <c r="F211" s="1"/>
-    </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D211" s="1">
+        <v>45801.345138888886</v>
+      </c>
+      <c r="E211" s="1">
+        <v>45801.53125</v>
+      </c>
+      <c r="F211" s="1">
+        <f t="shared" si="12"/>
+        <v>45801.438194444447</v>
+      </c>
+      <c r="G211">
+        <f t="shared" si="10"/>
+        <v>11.604861111110949</v>
+      </c>
+      <c r="I211">
+        <v>7.61</v>
+      </c>
+      <c r="J211">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="212" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A212">
         <v>53</v>
       </c>
@@ -14273,9 +14478,28 @@
         <f t="shared" si="11"/>
         <v>F3-53</v>
       </c>
-      <c r="F212" s="1"/>
-    </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D212" s="1">
+        <v>45801.345138888886</v>
+      </c>
+      <c r="E212" s="1">
+        <v>45801.53125</v>
+      </c>
+      <c r="F212" s="1">
+        <f t="shared" si="12"/>
+        <v>45801.438194444447</v>
+      </c>
+      <c r="G212">
+        <f t="shared" si="10"/>
+        <v>11.595138888893416</v>
+      </c>
+      <c r="I212">
+        <v>7.55</v>
+      </c>
+      <c r="J212">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="213" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A213">
         <v>53</v>
       </c>
@@ -14286,9 +14510,28 @@
         <f t="shared" si="11"/>
         <v>F4-53</v>
       </c>
-      <c r="F213" s="1"/>
-    </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D213" s="1">
+        <v>45801.345138888886</v>
+      </c>
+      <c r="E213" s="1">
+        <v>45801.53125</v>
+      </c>
+      <c r="F213" s="1">
+        <f t="shared" si="12"/>
+        <v>45801.438194444447</v>
+      </c>
+      <c r="G213">
+        <f t="shared" si="10"/>
+        <v>11.595138888893416</v>
+      </c>
+      <c r="I213">
+        <v>7.64</v>
+      </c>
+      <c r="J213">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="214" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A214">
         <v>54</v>
       </c>
@@ -14299,9 +14542,22 @@
         <f t="shared" si="11"/>
         <v>F1-54</v>
       </c>
-      <c r="F214" s="1"/>
-    </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D214" s="1">
+        <v>45801.53402777778</v>
+      </c>
+      <c r="E214" s="1">
+        <v>45801.55972222222</v>
+      </c>
+      <c r="F214" s="1">
+        <f t="shared" si="12"/>
+        <v>45801.546875</v>
+      </c>
+      <c r="G214">
+        <f t="shared" si="10"/>
+        <v>11.713541666664241</v>
+      </c>
+    </row>
+    <row r="215" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A215">
         <v>54</v>
       </c>
@@ -14312,9 +14568,22 @@
         <f t="shared" si="11"/>
         <v>F2-54</v>
       </c>
-      <c r="F215" s="1"/>
-    </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D215" s="1">
+        <v>45801.53402777778</v>
+      </c>
+      <c r="E215" s="1">
+        <v>45801.55972222222</v>
+      </c>
+      <c r="F215" s="1">
+        <f t="shared" si="12"/>
+        <v>45801.546875</v>
+      </c>
+      <c r="G215">
+        <f t="shared" si="10"/>
+        <v>11.713541666664241</v>
+      </c>
+    </row>
+    <row r="216" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A216">
         <v>54</v>
       </c>
@@ -14325,9 +14594,22 @@
         <f t="shared" si="11"/>
         <v>F3-54</v>
       </c>
-      <c r="F216" s="1"/>
-    </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D216" s="1">
+        <v>45801.53402777778</v>
+      </c>
+      <c r="E216" s="1">
+        <v>45801.55972222222</v>
+      </c>
+      <c r="F216" s="1">
+        <f t="shared" si="12"/>
+        <v>45801.546875</v>
+      </c>
+      <c r="G216">
+        <f t="shared" si="10"/>
+        <v>11.703819444446708</v>
+      </c>
+    </row>
+    <row r="217" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A217">
         <v>54</v>
       </c>
@@ -14338,7 +14620,563 @@
         <f t="shared" si="11"/>
         <v>F4-54</v>
       </c>
-      <c r="F217" s="1"/>
+      <c r="D217" s="1">
+        <v>45801.53402777778</v>
+      </c>
+      <c r="E217" s="1">
+        <v>45801.55972222222</v>
+      </c>
+      <c r="F217" s="1">
+        <f t="shared" si="12"/>
+        <v>45801.546875</v>
+      </c>
+      <c r="G217">
+        <f t="shared" si="10"/>
+        <v>11.703819444446708</v>
+      </c>
+    </row>
+    <row r="218" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A218">
+        <v>55</v>
+      </c>
+      <c r="B218" s="2">
+        <v>1</v>
+      </c>
+      <c r="C218" t="str">
+        <f t="shared" si="11"/>
+        <v>F1-55</v>
+      </c>
+      <c r="D218" s="1">
+        <v>45801.5625</v>
+      </c>
+      <c r="E218" s="3">
+        <v>45801.791666666664</v>
+      </c>
+      <c r="F218" s="1">
+        <f t="shared" si="12"/>
+        <v>45801.677083333328</v>
+      </c>
+      <c r="G218">
+        <f t="shared" si="10"/>
+        <v>11.843749999992724</v>
+      </c>
+      <c r="H218">
+        <v>32.1</v>
+      </c>
+      <c r="I218">
+        <v>7.35</v>
+      </c>
+      <c r="J218">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="219" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A219">
+        <v>55</v>
+      </c>
+      <c r="B219" s="2">
+        <v>2</v>
+      </c>
+      <c r="C219" t="str">
+        <f t="shared" si="11"/>
+        <v>F2-55</v>
+      </c>
+      <c r="D219" s="1">
+        <v>45801.5625</v>
+      </c>
+      <c r="E219" s="3">
+        <v>45801.791666666664</v>
+      </c>
+      <c r="F219" s="1">
+        <f t="shared" si="12"/>
+        <v>45801.677083333328</v>
+      </c>
+      <c r="G219">
+        <f t="shared" si="10"/>
+        <v>11.843749999992724</v>
+      </c>
+      <c r="H219">
+        <v>33.5</v>
+      </c>
+      <c r="I219">
+        <v>7.31</v>
+      </c>
+      <c r="J219">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="220" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A220">
+        <v>55</v>
+      </c>
+      <c r="B220" s="2">
+        <v>3</v>
+      </c>
+      <c r="C220" t="str">
+        <f t="shared" si="11"/>
+        <v>F3-55</v>
+      </c>
+      <c r="D220" s="1">
+        <v>45801.5625</v>
+      </c>
+      <c r="E220" s="3">
+        <v>45801.791666666664</v>
+      </c>
+      <c r="F220" s="1">
+        <f t="shared" si="12"/>
+        <v>45801.677083333328</v>
+      </c>
+      <c r="G220">
+        <f t="shared" si="10"/>
+        <v>11.834027777775191</v>
+      </c>
+      <c r="H220">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="I220">
+        <v>7.33</v>
+      </c>
+      <c r="J220">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="221" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A221">
+        <v>55</v>
+      </c>
+      <c r="B221" s="2">
+        <v>4</v>
+      </c>
+      <c r="C221" t="str">
+        <f t="shared" si="11"/>
+        <v>F4-55</v>
+      </c>
+      <c r="D221" s="1">
+        <v>45801.5625</v>
+      </c>
+      <c r="E221" s="3">
+        <v>45801.791666666664</v>
+      </c>
+      <c r="F221" s="1">
+        <f t="shared" si="12"/>
+        <v>45801.677083333328</v>
+      </c>
+      <c r="G221">
+        <f t="shared" si="10"/>
+        <v>11.834027777775191</v>
+      </c>
+      <c r="H221">
+        <v>33.4</v>
+      </c>
+      <c r="I221">
+        <v>7.31</v>
+      </c>
+      <c r="J221">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="222" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A222">
+        <v>56</v>
+      </c>
+      <c r="B222" s="2">
+        <v>1</v>
+      </c>
+      <c r="C222" t="str">
+        <f t="shared" si="11"/>
+        <v>F1-56</v>
+      </c>
+      <c r="D222" s="1">
+        <v>45801.792361111111</v>
+      </c>
+      <c r="E222" s="1">
+        <v>45802.385416666664</v>
+      </c>
+      <c r="F222" s="1">
+        <f t="shared" si="12"/>
+        <v>45802.088888888888</v>
+      </c>
+      <c r="G222">
+        <f t="shared" si="10"/>
+        <v>12.255555555551837</v>
+      </c>
+    </row>
+    <row r="223" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A223">
+        <v>56</v>
+      </c>
+      <c r="B223" s="2">
+        <v>2</v>
+      </c>
+      <c r="C223" t="str">
+        <f t="shared" si="11"/>
+        <v>F2-56</v>
+      </c>
+      <c r="D223" s="1">
+        <v>45801.792361111111</v>
+      </c>
+      <c r="E223" s="1">
+        <v>45802.385416666664</v>
+      </c>
+      <c r="F223" s="1">
+        <f t="shared" si="12"/>
+        <v>45802.088888888888</v>
+      </c>
+      <c r="G223">
+        <f t="shared" si="10"/>
+        <v>12.255555555551837</v>
+      </c>
+    </row>
+    <row r="224" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A224">
+        <v>56</v>
+      </c>
+      <c r="B224" s="2">
+        <v>3</v>
+      </c>
+      <c r="C224" t="str">
+        <f t="shared" si="11"/>
+        <v>F3-56</v>
+      </c>
+      <c r="D224" s="1">
+        <v>45801.792361111111</v>
+      </c>
+      <c r="E224" s="1">
+        <v>45802.385416666664</v>
+      </c>
+      <c r="F224" s="1">
+        <f t="shared" si="12"/>
+        <v>45802.088888888888</v>
+      </c>
+      <c r="G224">
+        <f t="shared" si="10"/>
+        <v>12.245833333334303</v>
+      </c>
+    </row>
+    <row r="225" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A225">
+        <v>56</v>
+      </c>
+      <c r="B225" s="2">
+        <v>4</v>
+      </c>
+      <c r="C225" t="str">
+        <f t="shared" si="11"/>
+        <v>F4-56</v>
+      </c>
+      <c r="D225" s="1">
+        <v>45801.792361111111</v>
+      </c>
+      <c r="E225" s="1">
+        <v>45802.385416666664</v>
+      </c>
+      <c r="F225" s="1">
+        <f t="shared" si="12"/>
+        <v>45802.088888888888</v>
+      </c>
+      <c r="G225">
+        <f t="shared" si="10"/>
+        <v>12.245833333334303</v>
+      </c>
+    </row>
+    <row r="226" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A226">
+        <v>57</v>
+      </c>
+      <c r="B226" s="2">
+        <v>1</v>
+      </c>
+      <c r="C226" t="str">
+        <f t="shared" si="11"/>
+        <v>F1-57</v>
+      </c>
+      <c r="D226" s="1">
+        <v>45802.387499999997</v>
+      </c>
+      <c r="E226" s="1">
+        <v>45802.540972222225</v>
+      </c>
+      <c r="F226" s="1">
+        <f t="shared" si="12"/>
+        <v>45802.464236111111</v>
+      </c>
+      <c r="G226">
+        <f t="shared" si="10"/>
+        <v>12.630902777775191</v>
+      </c>
+      <c r="H226">
+        <v>32.1</v>
+      </c>
+      <c r="I226">
+        <v>7.44</v>
+      </c>
+      <c r="J226">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="227" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A227">
+        <v>57</v>
+      </c>
+      <c r="B227" s="2">
+        <v>2</v>
+      </c>
+      <c r="C227" t="str">
+        <f t="shared" si="11"/>
+        <v>F2-57</v>
+      </c>
+      <c r="D227" s="1">
+        <v>45802.387499999997</v>
+      </c>
+      <c r="E227" s="1">
+        <v>45802.540972222225</v>
+      </c>
+      <c r="F227" s="1">
+        <f t="shared" si="12"/>
+        <v>45802.464236111111</v>
+      </c>
+      <c r="G227">
+        <f t="shared" si="10"/>
+        <v>12.630902777775191</v>
+      </c>
+      <c r="H227">
+        <v>33.1</v>
+      </c>
+      <c r="I227">
+        <v>7.44</v>
+      </c>
+      <c r="J227">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="228" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A228">
+        <v>57</v>
+      </c>
+      <c r="B228" s="2">
+        <v>3</v>
+      </c>
+      <c r="C228" t="str">
+        <f t="shared" si="11"/>
+        <v>F3-57</v>
+      </c>
+      <c r="D228" s="1">
+        <v>45802.387499999997</v>
+      </c>
+      <c r="E228" s="1">
+        <v>45802.540972222225</v>
+      </c>
+      <c r="F228" s="1">
+        <f t="shared" si="12"/>
+        <v>45802.464236111111</v>
+      </c>
+      <c r="G228">
+        <f t="shared" si="10"/>
+        <v>12.621180555557657</v>
+      </c>
+      <c r="H228">
+        <v>33.9</v>
+      </c>
+      <c r="I228">
+        <v>7.42</v>
+      </c>
+      <c r="J228">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="229" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A229">
+        <v>57</v>
+      </c>
+      <c r="B229" s="2">
+        <v>4</v>
+      </c>
+      <c r="C229" t="str">
+        <f t="shared" si="11"/>
+        <v>F4-57</v>
+      </c>
+      <c r="D229" s="1">
+        <v>45802.387499999997</v>
+      </c>
+      <c r="E229" s="1">
+        <v>45802.540972222225</v>
+      </c>
+      <c r="F229" s="1">
+        <f t="shared" si="12"/>
+        <v>45802.464236111111</v>
+      </c>
+      <c r="G229">
+        <f t="shared" si="10"/>
+        <v>12.621180555557657</v>
+      </c>
+    </row>
+    <row r="230" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A230">
+        <v>58</v>
+      </c>
+      <c r="B230" s="2">
+        <v>1</v>
+      </c>
+      <c r="C230" t="str">
+        <f t="shared" si="11"/>
+        <v>F1-58</v>
+      </c>
+      <c r="D230" s="1">
+        <v>45802.542361111111</v>
+      </c>
+      <c r="F230" s="1"/>
+    </row>
+    <row r="231" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A231">
+        <v>58</v>
+      </c>
+      <c r="B231" s="2">
+        <v>2</v>
+      </c>
+      <c r="C231" t="str">
+        <f t="shared" si="11"/>
+        <v>F2-58</v>
+      </c>
+      <c r="D231" s="1">
+        <v>45802.542361111111</v>
+      </c>
+      <c r="F231" s="1"/>
+    </row>
+    <row r="232" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A232">
+        <v>58</v>
+      </c>
+      <c r="B232" s="2">
+        <v>3</v>
+      </c>
+      <c r="C232" t="str">
+        <f t="shared" si="11"/>
+        <v>F3-58</v>
+      </c>
+      <c r="D232" s="1">
+        <v>45802.542361111111</v>
+      </c>
+      <c r="F232" s="1"/>
+    </row>
+    <row r="233" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A233">
+        <v>58</v>
+      </c>
+      <c r="B233" s="2">
+        <v>4</v>
+      </c>
+      <c r="C233" t="str">
+        <f t="shared" si="11"/>
+        <v>F4-58</v>
+      </c>
+      <c r="D233" s="1">
+        <v>45802.542361111111</v>
+      </c>
+      <c r="F233" s="1"/>
+    </row>
+    <row r="234" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A234">
+        <v>59</v>
+      </c>
+      <c r="B234" s="2">
+        <v>1</v>
+      </c>
+      <c r="C234" t="str">
+        <f t="shared" si="11"/>
+        <v>F1-59</v>
+      </c>
+      <c r="F234" s="1"/>
+    </row>
+    <row r="235" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A235">
+        <v>59</v>
+      </c>
+      <c r="B235" s="2">
+        <v>2</v>
+      </c>
+      <c r="C235" t="str">
+        <f t="shared" si="11"/>
+        <v>F2-59</v>
+      </c>
+      <c r="F235" s="1"/>
+    </row>
+    <row r="236" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A236">
+        <v>59</v>
+      </c>
+      <c r="B236" s="2">
+        <v>3</v>
+      </c>
+      <c r="C236" t="str">
+        <f t="shared" si="11"/>
+        <v>F3-59</v>
+      </c>
+      <c r="F236" s="1"/>
+    </row>
+    <row r="237" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A237">
+        <v>59</v>
+      </c>
+      <c r="B237" s="2">
+        <v>4</v>
+      </c>
+      <c r="C237" t="str">
+        <f t="shared" si="11"/>
+        <v>F4-59</v>
+      </c>
+      <c r="F237" s="1"/>
+    </row>
+    <row r="238" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A238">
+        <v>60</v>
+      </c>
+      <c r="B238" s="2">
+        <v>1</v>
+      </c>
+      <c r="C238" t="str">
+        <f t="shared" si="11"/>
+        <v>F1-60</v>
+      </c>
+      <c r="F238" s="1"/>
+    </row>
+    <row r="239" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A239">
+        <v>60</v>
+      </c>
+      <c r="B239" s="2">
+        <v>2</v>
+      </c>
+      <c r="C239" t="str">
+        <f t="shared" si="11"/>
+        <v>F2-60</v>
+      </c>
+      <c r="F239" s="1"/>
+    </row>
+    <row r="240" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A240">
+        <v>60</v>
+      </c>
+      <c r="B240" s="2">
+        <v>3</v>
+      </c>
+      <c r="C240" t="str">
+        <f t="shared" si="11"/>
+        <v>F3-60</v>
+      </c>
+      <c r="F240" s="1"/>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A241">
+        <v>60</v>
+      </c>
+      <c r="B241" s="2">
+        <v>4</v>
+      </c>
+      <c r="C241" t="str">
+        <f t="shared" si="11"/>
+        <v>F4-60</v>
+      </c>
+      <c r="F241" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
data updates from latest ic results, plus changes in boundary conditions
</commit_message>
<xml_diff>
--- a/data/exp_raw/no2_analyticall_results.xlsx
+++ b/data/exp_raw/no2_analyticall_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vcantarella/Documents/FuhrbergerColumns/data/exp_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACDB4E68-D55B-A14C-9D8C-163CFC3B3D03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080B30E0-6C4D-4F4E-9E6E-67D9C2B682D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="740" windowWidth="28040" windowHeight="16680" firstSheet="1" activeTab="6" xr2:uid="{3CD87C21-EA08-D841-BE93-D5199CA9A403}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="164">
   <si>
     <t>Standard</t>
   </si>
@@ -395,6 +395,147 @@
   </si>
   <si>
     <t>dil 5x</t>
+  </si>
+  <si>
+    <t>008-F1-62</t>
+  </si>
+  <si>
+    <t>009-F2-62</t>
+  </si>
+  <si>
+    <t>010-F3-62</t>
+  </si>
+  <si>
+    <t>011-F4-62</t>
+  </si>
+  <si>
+    <t>012-F1-59</t>
+  </si>
+  <si>
+    <t>013-F2-59</t>
+  </si>
+  <si>
+    <t>014-F3-59</t>
+  </si>
+  <si>
+    <t>015-F4-59</t>
+  </si>
+  <si>
+    <t>016-F1-57</t>
+  </si>
+  <si>
+    <t>017-F2-57</t>
+  </si>
+  <si>
+    <t>018-F3-57</t>
+  </si>
+  <si>
+    <t>019-F1-56</t>
+  </si>
+  <si>
+    <t>020-F2-56</t>
+  </si>
+  <si>
+    <t>021-F3-56</t>
+  </si>
+  <si>
+    <t>022-F4-56</t>
+  </si>
+  <si>
+    <t>023-F1-55</t>
+  </si>
+  <si>
+    <t>024-F2-55</t>
+  </si>
+  <si>
+    <t>025-F3-55</t>
+  </si>
+  <si>
+    <t>026-F4-55</t>
+  </si>
+  <si>
+    <t>027-F1-53</t>
+  </si>
+  <si>
+    <t>028-F2-53</t>
+  </si>
+  <si>
+    <t>029-F3-53</t>
+  </si>
+  <si>
+    <t>030-F4-53</t>
+  </si>
+  <si>
+    <t>031-F1-49</t>
+  </si>
+  <si>
+    <t>032-F2-49</t>
+  </si>
+  <si>
+    <t>033-F3-49</t>
+  </si>
+  <si>
+    <t>034-F4-49</t>
+  </si>
+  <si>
+    <t>035-F1-51</t>
+  </si>
+  <si>
+    <t>036-F2-51</t>
+  </si>
+  <si>
+    <t>037-F3-51</t>
+  </si>
+  <si>
+    <t>038-F4-51</t>
+  </si>
+  <si>
+    <t>039-F1-52</t>
+  </si>
+  <si>
+    <t>040-F2-52</t>
+  </si>
+  <si>
+    <t>041-F3-52</t>
+  </si>
+  <si>
+    <t>042-F4-52</t>
+  </si>
+  <si>
+    <t>043-F1-48</t>
+  </si>
+  <si>
+    <t>044-F2-48</t>
+  </si>
+  <si>
+    <t>045-F3-48</t>
+  </si>
+  <si>
+    <t>046-F4-48</t>
+  </si>
+  <si>
+    <t>047-F1-45</t>
+  </si>
+  <si>
+    <t>048-F2-45</t>
+  </si>
+  <si>
+    <t>049-F3-45</t>
+  </si>
+  <si>
+    <t>050-F4-45</t>
+  </si>
+  <si>
+    <t>051-F1-44</t>
+  </si>
+  <si>
+    <t>052-F2-44</t>
+  </si>
+  <si>
+    <t>053-F3-44</t>
+  </si>
+  <si>
+    <t>054-F4-44</t>
   </si>
 </sst>
 </file>
@@ -12443,8 +12584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28553D95-A703-174C-8A27-2C251D35502B}">
   <dimension ref="A1:P465"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A307" zoomScale="110" workbookViewId="0">
-      <selection activeCell="K329" sqref="K318:K329"/>
+    <sheetView tabSelected="1" topLeftCell="B90" zoomScale="110" workbookViewId="0">
+      <selection activeCell="M166" sqref="M166:N173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18103,11 +18244,11 @@
         <v>8.2059027777795563</v>
       </c>
       <c r="M165">
-        <f>VLOOKUP(C165,Sheet1!$B$3:$E$73,4,FALSE)/62*1000</f>
+        <f>VLOOKUP(C165,Sheet1!$B$3:$E$400,4,FALSE)/62*1000</f>
         <v>2.4991583075564319</v>
       </c>
       <c r="N165">
-        <f>VLOOKUP(C165,Sheet1!$B$3:$E$73,3,FALSE)/96*1000</f>
+        <f>VLOOKUP(C165,Sheet1!$B$3:$E$400,3,FALSE)/96*1000</f>
         <v>2592.8394239710155</v>
       </c>
     </row>
@@ -18360,6 +18501,14 @@
         <f>VLOOKUP(sampling!C174,standard_curve_plate_3!$C$2:$G$49,5,FALSE)</f>
         <v>0.18348999999999993</v>
       </c>
+      <c r="M174">
+        <f>VLOOKUP(C174,Sheet1!$B$3:$E$400,4,FALSE)/62*1000</f>
+        <v>2.2560459419753034</v>
+      </c>
+      <c r="N174">
+        <f>VLOOKUP(C174,Sheet1!$B$3:$E$400,3,FALSE)/96*1000</f>
+        <v>2595.432789510895</v>
+      </c>
     </row>
     <row r="175" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A175">
@@ -18390,6 +18539,14 @@
         <f>VLOOKUP(sampling!C175,standard_curve_plate_3!$C$2:$G$49,5,FALSE)</f>
         <v>-0.48492999999999942</v>
       </c>
+      <c r="M175">
+        <f>VLOOKUP(C175,Sheet1!$B$3:$E$400,4,FALSE)/62*1000</f>
+        <v>2.2132865522086966</v>
+      </c>
+      <c r="N175">
+        <f>VLOOKUP(C175,Sheet1!$B$3:$E$400,3,FALSE)/96*1000</f>
+        <v>2633.7492929260411</v>
+      </c>
     </row>
     <row r="176" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A176">
@@ -18420,8 +18577,16 @@
         <f>VLOOKUP(sampling!C176,standard_curve_plate_3!$C$2:$G$49,5,FALSE)</f>
         <v>-1.7035999999999607E-2</v>
       </c>
-    </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M176">
+        <f>VLOOKUP(C176,Sheet1!$B$3:$E$400,4,FALSE)/62*1000</f>
+        <v>1.8269213011753018</v>
+      </c>
+      <c r="N176">
+        <f>VLOOKUP(C176,Sheet1!$B$3:$E$400,3,FALSE)/96*1000</f>
+        <v>2609.8229437625782</v>
+      </c>
+    </row>
+    <row r="177" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>44</v>
       </c>
@@ -18450,8 +18615,16 @@
         <f>VLOOKUP(sampling!C177,standard_curve_plate_3!$C$2:$G$49,5,FALSE)</f>
         <v>-0.68545599999999984</v>
       </c>
-    </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M177">
+        <f>VLOOKUP(C177,Sheet1!$B$3:$E$400,4,FALSE)/62*1000</f>
+        <v>2.9132221688910516</v>
+      </c>
+      <c r="N177">
+        <f>VLOOKUP(C177,Sheet1!$B$3:$E$400,3,FALSE)/96*1000</f>
+        <v>2618.0383710692199</v>
+      </c>
+    </row>
+    <row r="178" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>45</v>
       </c>
@@ -18479,8 +18652,16 @@
       <c r="H178">
         <v>31.2</v>
       </c>
-    </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M178">
+        <f>VLOOKUP(C178,Sheet1!$B$3:$E$400,4,FALSE)/62*1000</f>
+        <v>2.2199679899192373</v>
+      </c>
+      <c r="N178">
+        <f>VLOOKUP(C178,Sheet1!$B$3:$E$400,3,FALSE)/96*1000</f>
+        <v>2596.0142687393072</v>
+      </c>
+    </row>
+    <row r="179" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>45</v>
       </c>
@@ -18508,8 +18689,16 @@
       <c r="H179">
         <v>32.200000000000003</v>
       </c>
-    </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M179">
+        <f>VLOOKUP(C179,Sheet1!$B$3:$E$400,4,FALSE)/62*1000</f>
+        <v>2.2159591398733354</v>
+      </c>
+      <c r="N179">
+        <f>VLOOKUP(C179,Sheet1!$B$3:$E$400,3,FALSE)/96*1000</f>
+        <v>2599.7796455056814</v>
+      </c>
+    </row>
+    <row r="180" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>45</v>
       </c>
@@ -18537,8 +18726,16 @@
       <c r="H180">
         <v>32.6</v>
       </c>
-    </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M180">
+        <f>VLOOKUP(C180,Sheet1!$B$3:$E$400,4,FALSE)/62*1000</f>
+        <v>2.2413478860893017</v>
+      </c>
+      <c r="N180">
+        <f>VLOOKUP(C180,Sheet1!$B$3:$E$400,3,FALSE)/96*1000</f>
+        <v>2606.4727823550188</v>
+      </c>
+    </row>
+    <row r="181" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>45</v>
       </c>
@@ -18566,8 +18763,16 @@
       <c r="H181">
         <v>31.5</v>
       </c>
-    </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M181">
+        <f>VLOOKUP(C181,Sheet1!$B$3:$E$400,4,FALSE)/62*1000</f>
+        <v>3.4049286483412509</v>
+      </c>
+      <c r="N181">
+        <f>VLOOKUP(C181,Sheet1!$B$3:$E$400,3,FALSE)/96*1000</f>
+        <v>2629.7920847530577</v>
+      </c>
+    </row>
+    <row r="182" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>46</v>
       </c>
@@ -18593,7 +18798,7 @@
         <v>9.5930555555532919</v>
       </c>
     </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>46</v>
       </c>
@@ -18619,7 +18824,7 @@
         <v>9.5930555555532919</v>
       </c>
     </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>46</v>
       </c>
@@ -18645,7 +18850,7 @@
         <v>9.5833333333357587</v>
       </c>
     </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>46</v>
       </c>
@@ -18671,7 +18876,7 @@
         <v>9.5833333333357587</v>
       </c>
     </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>47</v>
       </c>
@@ -18701,7 +18906,7 @@
         <v>19.4648</v>
       </c>
     </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>47</v>
       </c>
@@ -18731,7 +18936,7 @@
         <v>46.692800000000005</v>
       </c>
     </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>47</v>
       </c>
@@ -18761,7 +18966,7 @@
         <v>27.633199999999999</v>
       </c>
     </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>47</v>
       </c>
@@ -18791,7 +18996,7 @@
         <v>5.8508000000000031</v>
       </c>
     </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>48</v>
       </c>
@@ -18825,8 +19030,16 @@
       <c r="J190">
         <v>1032</v>
       </c>
-    </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M190">
+        <f>VLOOKUP(C190,Sheet1!$B$3:$E$400,4,FALSE)/62*1000</f>
+        <v>1.9766961129667335</v>
+      </c>
+      <c r="N190">
+        <f>VLOOKUP(C190,Sheet1!$B$3:$E$400,3,FALSE)/96*1000</f>
+        <v>2584.094723764415</v>
+      </c>
+    </row>
+    <row r="191" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>48</v>
       </c>
@@ -18860,8 +19073,16 @@
       <c r="J191">
         <v>1010</v>
       </c>
-    </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M191">
+        <f>VLOOKUP(C191,Sheet1!$B$3:$E$400,4,FALSE)/62*1000</f>
+        <v>1.8844303517213352</v>
+      </c>
+      <c r="N191">
+        <f>VLOOKUP(C191,Sheet1!$B$3:$E$400,3,FALSE)/96*1000</f>
+        <v>2591.0502612336286</v>
+      </c>
+    </row>
+    <row r="192" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>48</v>
       </c>
@@ -18895,8 +19116,16 @@
       <c r="J192">
         <v>1093</v>
       </c>
-    </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M192">
+        <f>VLOOKUP(C192,Sheet1!$B$3:$E$400,4,FALSE)/62*1000</f>
+        <v>2.3535747283905275</v>
+      </c>
+      <c r="N192">
+        <f>VLOOKUP(C192,Sheet1!$B$3:$E$400,3,FALSE)/96*1000</f>
+        <v>2602.4728041359408</v>
+      </c>
+    </row>
+    <row r="193" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>48</v>
       </c>
@@ -18930,8 +19159,16 @@
       <c r="J193">
         <v>888</v>
       </c>
-    </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M193">
+        <f>VLOOKUP(C193,Sheet1!$B$3:$E$400,4,FALSE)/62*1000</f>
+        <v>2.318841010510166</v>
+      </c>
+      <c r="N193">
+        <f>VLOOKUP(C193,Sheet1!$B$3:$E$400,3,FALSE)/96*1000</f>
+        <v>2613.7856731347138</v>
+      </c>
+    </row>
+    <row r="194" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>49</v>
       </c>
@@ -18963,8 +19200,16 @@
         <f>VLOOKUP(sampling!C194,standard_curve_plate_3!$C$2:$G$49,5,FALSE)</f>
         <v>-0.21756200000000003</v>
       </c>
-    </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M194">
+        <f>VLOOKUP(C194,Sheet1!$B$3:$E$400,4,FALSE)/62*1000</f>
+        <v>1.9967512452617742</v>
+      </c>
+      <c r="N194">
+        <f>VLOOKUP(C194,Sheet1!$B$3:$E$400,3,FALSE)/96*1000</f>
+        <v>2595.1796986205854</v>
+      </c>
+    </row>
+    <row r="195" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>49</v>
       </c>
@@ -18996,8 +19241,16 @@
         <f>VLOOKUP(sampling!C195,standard_curve_plate_3!$C$2:$G$49,5,FALSE)</f>
         <v>-0.21756200000000003</v>
       </c>
-    </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M195">
+        <f>VLOOKUP(C195,Sheet1!$B$3:$E$400,4,FALSE)/62*1000</f>
+        <v>2.0903293870529027</v>
+      </c>
+      <c r="N195">
+        <f>VLOOKUP(C195,Sheet1!$B$3:$E$400,3,FALSE)/96*1000</f>
+        <v>2578.7102351368821</v>
+      </c>
+    </row>
+    <row r="196" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>49</v>
       </c>
@@ -19029,8 +19282,16 @@
         <f>VLOOKUP(sampling!C196,standard_curve_plate_3!$C$2:$G$49,5,FALSE)</f>
         <v>-0.35124600000000017</v>
       </c>
-    </row>
-    <row r="197" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M196">
+        <f>VLOOKUP(C196,Sheet1!$B$3:$E$400,4,FALSE)/62*1000</f>
+        <v>2.7221117355823341</v>
+      </c>
+      <c r="N196">
+        <f>VLOOKUP(C196,Sheet1!$B$3:$E$400,3,FALSE)/96*1000</f>
+        <v>2586.1208531249695</v>
+      </c>
+    </row>
+    <row r="197" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>49</v>
       </c>
@@ -19062,8 +19323,16 @@
         <f>VLOOKUP(sampling!C197,standard_curve_plate_3!$C$2:$G$204,5,FALSE)</f>
         <v>-0.68545599999999984</v>
       </c>
-    </row>
-    <row r="198" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M197">
+        <f>VLOOKUP(C197,Sheet1!$B$3:$E$400,4,FALSE)/62*1000</f>
+        <v>1.9700108591946774</v>
+      </c>
+      <c r="N197">
+        <f>VLOOKUP(C197,Sheet1!$B$3:$E$400,3,FALSE)/96*1000</f>
+        <v>2596.8274344724646</v>
+      </c>
+    </row>
+    <row r="198" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>50</v>
       </c>
@@ -19093,7 +19362,7 @@
         <v>22.868300000000001</v>
       </c>
     </row>
-    <row r="199" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>50</v>
       </c>
@@ -19123,7 +19392,7 @@
         <v>42.60860000000001</v>
       </c>
     </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>50</v>
       </c>
@@ -19153,7 +19422,7 @@
         <v>26.27180000000001</v>
       </c>
     </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A201">
         <v>50</v>
       </c>
@@ -19183,7 +19452,7 @@
         <v>3.8086999999999982</v>
       </c>
     </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>51</v>
       </c>
@@ -19221,8 +19490,16 @@
         <f>VLOOKUP(sampling!C202,standard_curve_plate_3!$C$2:$G$204,5,FALSE)</f>
         <v>-0.55177199999999971</v>
       </c>
-    </row>
-    <row r="203" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M202">
+        <f>VLOOKUP(C202,Sheet1!$B$3:$E$400,4,FALSE)/62*1000</f>
+        <v>2.0716154025365614</v>
+      </c>
+      <c r="N202">
+        <f>VLOOKUP(C202,Sheet1!$B$3:$E$400,3,FALSE)/96*1000</f>
+        <v>2493.0237806349987</v>
+      </c>
+    </row>
+    <row r="203" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A203">
         <v>51</v>
       </c>
@@ -19260,8 +19537,16 @@
         <f>VLOOKUP(sampling!C203,standard_curve_plate_3!$C$2:$G$204,5,FALSE)</f>
         <v>-0.21756200000000003</v>
       </c>
-    </row>
-    <row r="204" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M203">
+        <f>VLOOKUP(C203,Sheet1!$B$3:$E$400,4,FALSE)/62*1000</f>
+        <v>1.8255837891387292</v>
+      </c>
+      <c r="N203">
+        <f>VLOOKUP(C203,Sheet1!$B$3:$E$400,3,FALSE)/96*1000</f>
+        <v>2471.862143364423</v>
+      </c>
+    </row>
+    <row r="204" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A204">
         <v>51</v>
       </c>
@@ -19299,8 +19584,16 @@
         <f>VLOOKUP(sampling!C204,standard_curve_plate_3!$C$2:$G$204,5,FALSE)</f>
         <v>-0.55177199999999971</v>
       </c>
-    </row>
-    <row r="205" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M204">
+        <f>VLOOKUP(C204,Sheet1!$B$3:$E$400,4,FALSE)/62*1000</f>
+        <v>1.9740220240383339</v>
+      </c>
+      <c r="N204">
+        <f>VLOOKUP(C204,Sheet1!$B$3:$E$400,3,FALSE)/96*1000</f>
+        <v>2503.2731137102851</v>
+      </c>
+    </row>
+    <row r="205" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A205">
         <v>51</v>
       </c>
@@ -19338,8 +19631,16 @@
         <f>VLOOKUP(sampling!C205,standard_curve_plate_3!$C$2:$G$204,5,FALSE)</f>
         <v>-0.55177199999999971</v>
       </c>
-    </row>
-    <row r="206" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M205">
+        <f>VLOOKUP(C205,Sheet1!$B$3:$E$400,4,FALSE)/62*1000</f>
+        <v>1.7653914072471724</v>
+      </c>
+      <c r="N205">
+        <f>VLOOKUP(C205,Sheet1!$B$3:$E$400,3,FALSE)/96*1000</f>
+        <v>2512.1116271821638</v>
+      </c>
+    </row>
+    <row r="206" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A206">
         <v>52</v>
       </c>
@@ -19374,8 +19675,16 @@
         <f>VLOOKUP(sampling!C206,standard_curve_plate_3!$C$2:$G$204,5,FALSE)</f>
         <v>-0.15071999999999974</v>
       </c>
-    </row>
-    <row r="207" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M206">
+        <f>VLOOKUP(C206,Sheet1!$B$3:$E$400,4,FALSE)/62*1000</f>
+        <v>2.4070056820513015</v>
+      </c>
+      <c r="N206">
+        <f>VLOOKUP(C206,Sheet1!$B$3:$E$400,3,FALSE)/96*1000</f>
+        <v>2469.9322044324931</v>
+      </c>
+    </row>
+    <row r="207" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A207">
         <v>52</v>
       </c>
@@ -19413,8 +19722,16 @@
         <f>VLOOKUP(sampling!C207,standard_curve_plate_3!$C$2:$G$204,5,FALSE)</f>
         <v>-0.41808800000000002</v>
       </c>
-    </row>
-    <row r="208" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M207">
+        <f>VLOOKUP(C207,Sheet1!$B$3:$E$400,4,FALSE)/62*1000</f>
+        <v>2.3322004682497788</v>
+      </c>
+      <c r="N207">
+        <f>VLOOKUP(C207,Sheet1!$B$3:$E$400,3,FALSE)/96*1000</f>
+        <v>2428.6852608151949</v>
+      </c>
+    </row>
+    <row r="208" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A208">
         <v>52</v>
       </c>
@@ -19449,8 +19766,16 @@
         <f>VLOOKUP(sampling!C208,standard_curve_plate_3!$C$2:$G$204,5,FALSE)</f>
         <v>-0.35124600000000017</v>
       </c>
-    </row>
-    <row r="209" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M208">
+        <f>VLOOKUP(C208,Sheet1!$B$3:$E$400,4,FALSE)/62*1000</f>
+        <v>2.0127946717549867</v>
+      </c>
+      <c r="N208">
+        <f>VLOOKUP(C208,Sheet1!$B$3:$E$400,3,FALSE)/96*1000</f>
+        <v>2494.9794246095726</v>
+      </c>
+    </row>
+    <row r="209" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A209">
         <v>52</v>
       </c>
@@ -19485,8 +19810,16 @@
         <f>VLOOKUP(sampling!C209,standard_curve_plate_3!$C$2:$G$204,5,FALSE)</f>
         <v>-0.48492999999999942</v>
       </c>
-    </row>
-    <row r="210" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M209">
+        <f>VLOOKUP(C209,Sheet1!$B$3:$E$400,4,FALSE)/62*1000</f>
+        <v>2.3375441339283469</v>
+      </c>
+      <c r="N209">
+        <f>VLOOKUP(C209,Sheet1!$B$3:$E$400,3,FALSE)/96*1000</f>
+        <v>2469.4329440861734</v>
+      </c>
+    </row>
+    <row r="210" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A210">
         <v>53</v>
       </c>
@@ -19521,8 +19854,16 @@
         <f>VLOOKUP(sampling!C210,standard_curve_plate_3!$C$2:$G$204,5,FALSE)</f>
         <v>-0.48492999999999942</v>
       </c>
-    </row>
-    <row r="211" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M210">
+        <f>VLOOKUP(C210,Sheet1!$B$3:$E$400,4,FALSE)/62*1000</f>
+        <v>2.8595636234474324</v>
+      </c>
+      <c r="N210">
+        <f>VLOOKUP(C210,Sheet1!$B$3:$E$400,3,FALSE)/96*1000</f>
+        <v>2407.3204819862449</v>
+      </c>
+    </row>
+    <row r="211" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A211">
         <v>53</v>
       </c>
@@ -19557,8 +19898,16 @@
         <f>VLOOKUP(sampling!C211,standard_curve_plate_3!$C$2:$G$204,5,FALSE)</f>
         <v>-0.61861399999999955</v>
       </c>
-    </row>
-    <row r="212" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M211">
+        <f>VLOOKUP(C211,Sheet1!$B$3:$E$400,4,FALSE)/62*1000</f>
+        <v>2.0796357822583746</v>
+      </c>
+      <c r="N211">
+        <f>VLOOKUP(C211,Sheet1!$B$3:$E$400,3,FALSE)/96*1000</f>
+        <v>2400.6593497141871</v>
+      </c>
+    </row>
+    <row r="212" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A212">
         <v>53</v>
       </c>
@@ -19593,8 +19942,16 @@
         <f>VLOOKUP(sampling!C212,standard_curve_plate_3!$C$2:$G$204,5,FALSE)</f>
         <v>-0.48492999999999942</v>
       </c>
-    </row>
-    <row r="213" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M212">
+        <f>VLOOKUP(C212,Sheet1!$B$3:$E$400,4,FALSE)/62*1000</f>
+        <v>2.4964874979248513</v>
+      </c>
+      <c r="N212">
+        <f>VLOOKUP(C212,Sheet1!$B$3:$E$400,3,FALSE)/96*1000</f>
+        <v>2453.4775225025332</v>
+      </c>
+    </row>
+    <row r="213" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A213">
         <v>53</v>
       </c>
@@ -19629,8 +19986,16 @@
         <f>VLOOKUP(sampling!C213,standard_curve_plate_3!$C$2:$G$204,5,FALSE)</f>
         <v>-0.68545599999999984</v>
       </c>
-    </row>
-    <row r="214" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M213">
+        <f>VLOOKUP(C213,Sheet1!$B$3:$E$400,4,FALSE)/62*1000</f>
+        <v>2.320176975154761</v>
+      </c>
+      <c r="N213">
+        <f>VLOOKUP(C213,Sheet1!$B$3:$E$400,3,FALSE)/96*1000</f>
+        <v>2450.5092759463687</v>
+      </c>
+    </row>
+    <row r="214" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A214">
         <v>54</v>
       </c>
@@ -19660,7 +20025,7 @@
         <v>19.4648</v>
       </c>
     </row>
-    <row r="215" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A215">
         <v>54</v>
       </c>
@@ -19690,7 +20055,7 @@
         <v>38.5244</v>
       </c>
     </row>
-    <row r="216" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A216">
         <v>54</v>
       </c>
@@ -19720,7 +20085,7 @@
         <v>18.784099999999999</v>
       </c>
     </row>
-    <row r="217" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A217">
         <v>54</v>
       </c>
@@ -19750,7 +20115,7 @@
         <v>4.4893999999999998</v>
       </c>
     </row>
-    <row r="218" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A218">
         <v>55</v>
       </c>
@@ -19788,8 +20153,16 @@
         <f>VLOOKUP(sampling!C218,standard_curve_plate_3!$C$2:$G$204,5,FALSE)</f>
         <v>-0.48492999999999942</v>
       </c>
-    </row>
-    <row r="219" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M218">
+        <f>VLOOKUP(C218,Sheet1!$B$3:$E$400,4,FALSE)/62*1000</f>
+        <v>2.9262718008188835</v>
+      </c>
+      <c r="N218">
+        <f>VLOOKUP(C218,Sheet1!$B$3:$E$400,3,FALSE)/96*1000</f>
+        <v>2384.9372021792346</v>
+      </c>
+    </row>
+    <row r="219" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A219">
         <v>55</v>
       </c>
@@ -19827,8 +20200,16 @@
         <f>VLOOKUP(sampling!C219,standard_curve_plate_3!$C$2:$G$204,5,FALSE)</f>
         <v>-0.61861399999999955</v>
       </c>
-    </row>
-    <row r="220" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M219">
+        <f>VLOOKUP(C219,Sheet1!$B$3:$E$400,4,FALSE)/62*1000</f>
+        <v>2.0261637325505033</v>
+      </c>
+      <c r="N219">
+        <f>VLOOKUP(C219,Sheet1!$B$3:$E$400,3,FALSE)/96*1000</f>
+        <v>2390.5610430039337</v>
+      </c>
+    </row>
+    <row r="220" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A220">
         <v>55</v>
       </c>
@@ -19866,8 +20247,16 @@
         <f>VLOOKUP(sampling!C220,standard_curve_plate_3!$C$2:$G$204,5,FALSE)</f>
         <v>-0.75229799999999969</v>
       </c>
-    </row>
-    <row r="221" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M220">
+        <f>VLOOKUP(C220,Sheet1!$B$3:$E$400,4,FALSE)/62*1000</f>
+        <v>2.2213042648809225</v>
+      </c>
+      <c r="N220">
+        <f>VLOOKUP(C220,Sheet1!$B$3:$E$400,3,FALSE)/96*1000</f>
+        <v>2447.8198701930373</v>
+      </c>
+    </row>
+    <row r="221" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A221">
         <v>55</v>
       </c>
@@ -19905,8 +20294,16 @@
         <f>VLOOKUP(sampling!C221,standard_curve_plate_3!$C$2:$G$204,5,FALSE)</f>
         <v>-0.68545599999999984</v>
       </c>
-    </row>
-    <row r="222" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M221">
+        <f>VLOOKUP(C221,Sheet1!$B$3:$E$400,4,FALSE)/62*1000</f>
+        <v>2.2760879277287471</v>
+      </c>
+      <c r="N221">
+        <f>VLOOKUP(C221,Sheet1!$B$3:$E$400,3,FALSE)/96*1000</f>
+        <v>2441.6309684921703</v>
+      </c>
+    </row>
+    <row r="222" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A222">
         <v>56</v>
       </c>
@@ -19935,8 +20332,16 @@
         <f>VLOOKUP(sampling!C222,standard_curve_plate_3!$C$2:$G$204,5,FALSE)</f>
         <v>-0.21756200000000003</v>
       </c>
-    </row>
-    <row r="223" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M222">
+        <f>VLOOKUP(C222,Sheet1!$B$3:$E$400,4,FALSE)/62*1000</f>
+        <v>3.5861171095459725</v>
+      </c>
+      <c r="N222">
+        <f>VLOOKUP(C222,Sheet1!$B$3:$E$400,3,FALSE)/96*1000</f>
+        <v>2383.7135323984971</v>
+      </c>
+    </row>
+    <row r="223" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A223">
         <v>56</v>
       </c>
@@ -19965,8 +20370,16 @@
         <f>VLOOKUP(sampling!C223,standard_curve_plate_3!$C$2:$G$204,5,FALSE)</f>
         <v>-0.41808800000000002</v>
       </c>
-    </row>
-    <row r="224" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M223">
+        <f>VLOOKUP(C223,Sheet1!$B$3:$E$400,4,FALSE)/62*1000</f>
+        <v>2.2239768022238713</v>
+      </c>
+      <c r="N223">
+        <f>VLOOKUP(C223,Sheet1!$B$3:$E$400,3,FALSE)/96*1000</f>
+        <v>2339.0962358815514</v>
+      </c>
+    </row>
+    <row r="224" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A224">
         <v>56</v>
       </c>
@@ -19995,8 +20408,16 @@
         <f>VLOOKUP(sampling!C224,standard_curve_plate_3!$C$2:$G$204,5,FALSE)</f>
         <v>-0.41808800000000002</v>
       </c>
-    </row>
-    <row r="225" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M224">
+        <f>VLOOKUP(C224,Sheet1!$B$3:$E$400,4,FALSE)/62*1000</f>
+        <v>2.4337186427971726</v>
+      </c>
+      <c r="N224">
+        <f>VLOOKUP(C224,Sheet1!$B$3:$E$400,3,FALSE)/96*1000</f>
+        <v>2446.2465704267529</v>
+      </c>
+    </row>
+    <row r="225" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A225">
         <v>56</v>
       </c>
@@ -20025,8 +20446,16 @@
         <f>VLOOKUP(sampling!C225,standard_curve_plate_3!$C$2:$G$204,5,FALSE)</f>
         <v>-0.68545599999999984</v>
       </c>
-    </row>
-    <row r="226" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M225">
+        <f>VLOOKUP(C225,Sheet1!$B$3:$E$400,4,FALSE)/62*1000</f>
+        <v>2.5352125958376241</v>
+      </c>
+      <c r="N225">
+        <f>VLOOKUP(C225,Sheet1!$B$3:$E$400,3,FALSE)/96*1000</f>
+        <v>2439.221881640131</v>
+      </c>
+    </row>
+    <row r="226" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A226">
         <v>57</v>
       </c>
@@ -20064,8 +20493,16 @@
         <f>VLOOKUP(sampling!C226,standard_curve_plate_3!$C$2:$G$204,5,FALSE)</f>
         <v>-0.61861399999999955</v>
       </c>
-    </row>
-    <row r="227" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M226">
+        <f>VLOOKUP(C226,Sheet1!$B$3:$E$400,4,FALSE)/62*1000</f>
+        <v>1.9593142350987289</v>
+      </c>
+      <c r="N226">
+        <f>VLOOKUP(C226,Sheet1!$B$3:$E$400,3,FALSE)/96*1000</f>
+        <v>2318.6746702610681</v>
+      </c>
+    </row>
+    <row r="227" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A227">
         <v>57</v>
       </c>
@@ -20103,8 +20540,16 @@
         <f>VLOOKUP(sampling!C227,standard_curve_plate_3!$C$2:$G$204,5,FALSE)</f>
         <v>-0.61861399999999955</v>
       </c>
-    </row>
-    <row r="228" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M227">
+        <f>VLOOKUP(C227,Sheet1!$B$3:$E$400,4,FALSE)/62*1000</f>
+        <v>2.0154685174618838</v>
+      </c>
+      <c r="N227">
+        <f>VLOOKUP(C227,Sheet1!$B$3:$E$400,3,FALSE)/96*1000</f>
+        <v>2312.1534302737055</v>
+      </c>
+    </row>
+    <row r="228" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A228">
         <v>57</v>
       </c>
@@ -20142,8 +20587,16 @@
         <f>VLOOKUP(sampling!C228,standard_curve_plate_3!$C$2:$G$204,5,FALSE)</f>
         <v>-0.41808800000000002</v>
       </c>
-    </row>
-    <row r="229" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M228">
+        <f>VLOOKUP(C228,Sheet1!$B$3:$E$400,4,FALSE)/62*1000</f>
+        <v>1.901815282438553</v>
+      </c>
+      <c r="N228">
+        <f>VLOOKUP(C228,Sheet1!$B$3:$E$400,3,FALSE)/96*1000</f>
+        <v>2419.5001225330752</v>
+      </c>
+    </row>
+    <row r="229" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A229">
         <v>57</v>
       </c>
@@ -20169,7 +20622,7 @@
         <v>12.621180555557657</v>
       </c>
     </row>
-    <row r="230" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A230">
         <v>58</v>
       </c>
@@ -20199,7 +20652,7 @@
         <v>26.27180000000001</v>
       </c>
     </row>
-    <row r="231" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A231">
         <v>58</v>
       </c>
@@ -20229,7 +20682,7 @@
         <v>53.499800000000008</v>
       </c>
     </row>
-    <row r="232" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A232">
         <v>58</v>
       </c>
@@ -20259,7 +20712,7 @@
         <v>22.868300000000001</v>
       </c>
     </row>
-    <row r="233" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A233">
         <v>58</v>
       </c>
@@ -20289,7 +20742,7 @@
         <v>3.8086999999999982</v>
       </c>
     </row>
-    <row r="234" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A234">
         <v>59</v>
       </c>
@@ -20318,8 +20771,16 @@
         <f>VLOOKUP(sampling!C234,standard_curve_plate_3!$C$2:$G$204,5,FALSE)</f>
         <v>-0.55177199999999971</v>
       </c>
-    </row>
-    <row r="235" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M234">
+        <f>VLOOKUP(C234,Sheet1!$B$3:$E$400,4,FALSE)/62*1000</f>
+        <v>2.1544853797907617</v>
+      </c>
+      <c r="N234">
+        <f>VLOOKUP(C234,Sheet1!$B$3:$E$400,3,FALSE)/96*1000</f>
+        <v>2324.097254335531</v>
+      </c>
+    </row>
+    <row r="235" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A235">
         <v>59</v>
       </c>
@@ -20348,8 +20809,16 @@
         <f>VLOOKUP(sampling!C235,standard_curve_plate_3!$C$2:$G$204,5,FALSE)</f>
         <v>-0.61861399999999955</v>
       </c>
-    </row>
-    <row r="236" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M235">
+        <f>VLOOKUP(C235,Sheet1!$B$3:$E$400,4,FALSE)/62*1000</f>
+        <v>1.6811078063997873</v>
+      </c>
+      <c r="N235">
+        <f>VLOOKUP(C235,Sheet1!$B$3:$E$400,3,FALSE)/96*1000</f>
+        <v>2281.8293894416624</v>
+      </c>
+    </row>
+    <row r="236" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A236">
         <v>59</v>
       </c>
@@ -20378,8 +20847,16 @@
         <f>VLOOKUP(sampling!C236,standard_curve_plate_3!$C$2:$G$204,5,FALSE)</f>
         <v>-0.35124600000000017</v>
       </c>
-    </row>
-    <row r="237" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M236">
+        <f>VLOOKUP(C236,Sheet1!$B$3:$E$400,4,FALSE)/62*1000</f>
+        <v>1.8603577392105033</v>
+      </c>
+      <c r="N236">
+        <f>VLOOKUP(C236,Sheet1!$B$3:$E$400,3,FALSE)/96*1000</f>
+        <v>2417.2678486219179</v>
+      </c>
+    </row>
+    <row r="237" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A237">
         <v>59</v>
       </c>
@@ -20408,8 +20885,16 @@
         <f>VLOOKUP(sampling!C237,standard_curve_plate_3!$C$2:$G$204,5,FALSE)</f>
         <v>-0.61861399999999955</v>
       </c>
-    </row>
-    <row r="238" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M237">
+        <f>VLOOKUP(C237,Sheet1!$B$3:$E$400,4,FALSE)/62*1000</f>
+        <v>1.7306097160220368</v>
+      </c>
+      <c r="N237">
+        <f>VLOOKUP(C237,Sheet1!$B$3:$E$400,3,FALSE)/96*1000</f>
+        <v>2420.1575191175425</v>
+      </c>
+    </row>
+    <row r="238" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A238">
         <v>60</v>
       </c>
@@ -20435,7 +20920,7 @@
         <v>13.277777777773736</v>
       </c>
     </row>
-    <row r="239" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A239">
         <v>60</v>
       </c>
@@ -20461,7 +20946,7 @@
         <v>13.277777777773736</v>
       </c>
     </row>
-    <row r="240" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A240">
         <v>60</v>
       </c>
@@ -20487,7 +20972,7 @@
         <v>13.268055555556202</v>
       </c>
     </row>
-    <row r="241" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A241">
         <v>60</v>
       </c>
@@ -20513,7 +20998,7 @@
         <v>13.268055555556202</v>
       </c>
     </row>
-    <row r="242" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A242">
         <v>61</v>
       </c>
@@ -20543,7 +21028,7 @@
         <v>26.952500000000011</v>
       </c>
     </row>
-    <row r="243" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A243">
         <v>61</v>
       </c>
@@ -20573,7 +21058,7 @@
         <v>48.054200000000009</v>
       </c>
     </row>
-    <row r="244" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A244">
         <v>61</v>
       </c>
@@ -20603,7 +21088,7 @@
         <v>19.4648</v>
       </c>
     </row>
-    <row r="245" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A245">
         <v>61</v>
       </c>
@@ -20633,7 +21118,7 @@
         <v>4.4893999999999998</v>
       </c>
     </row>
-    <row r="246" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A246">
         <v>62</v>
       </c>
@@ -20661,8 +21146,16 @@
       <c r="H246">
         <v>31.9</v>
       </c>
-    </row>
-    <row r="247" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M246">
+        <f>VLOOKUP(C246,Sheet1!$B$3:$E$400,4,FALSE)/62*1000</f>
+        <v>2.1478029146790432</v>
+      </c>
+      <c r="N246">
+        <f>VLOOKUP(C246,Sheet1!$B$3:$E$400,3,FALSE)/96*1000</f>
+        <v>2315.7333987237294</v>
+      </c>
+    </row>
+    <row r="247" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A247">
         <v>62</v>
       </c>
@@ -20690,8 +21183,16 @@
       <c r="H247">
         <v>31.9</v>
       </c>
-    </row>
-    <row r="248" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M247">
+        <f>VLOOKUP(C247,Sheet1!$B$3:$E$400,4,FALSE)/62*1000</f>
+        <v>2.3562464354255859</v>
+      </c>
+      <c r="N247">
+        <f>VLOOKUP(C247,Sheet1!$B$3:$E$400,3,FALSE)/96*1000</f>
+        <v>2247.1544913048738</v>
+      </c>
+    </row>
+    <row r="248" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A248">
         <v>62</v>
       </c>
@@ -20719,8 +21220,16 @@
       <c r="H248">
         <v>32.4</v>
       </c>
-    </row>
-    <row r="249" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M248">
+        <f>VLOOKUP(C248,Sheet1!$B$3:$E$400,4,FALSE)/62*1000</f>
+        <v>2.2881126662856004</v>
+      </c>
+      <c r="N248">
+        <f>VLOOKUP(C248,Sheet1!$B$3:$E$400,3,FALSE)/96*1000</f>
+        <v>2396.1979901785112</v>
+      </c>
+    </row>
+    <row r="249" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A249">
         <v>62</v>
       </c>
@@ -20748,8 +21257,16 @@
       <c r="H249">
         <v>31.9</v>
       </c>
-    </row>
-    <row r="250" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M249">
+        <f>VLOOKUP(C249,Sheet1!$B$3:$E$400,4,FALSE)/62*1000</f>
+        <v>1.9766961129667335</v>
+      </c>
+      <c r="N249">
+        <f>VLOOKUP(C249,Sheet1!$B$3:$E$400,3,FALSE)/96*1000</f>
+        <v>2403.8711907689913</v>
+      </c>
+    </row>
+    <row r="250" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A250">
         <v>63</v>
       </c>
@@ -20778,7 +21295,7 @@
         <v>32.17</v>
       </c>
     </row>
-    <row r="251" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A251">
         <v>63</v>
       </c>
@@ -20807,7 +21324,7 @@
         <v>32.299999999999997</v>
       </c>
     </row>
-    <row r="252" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A252">
         <v>63</v>
       </c>
@@ -20836,7 +21353,7 @@
         <v>32.200000000000003</v>
       </c>
     </row>
-    <row r="253" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A253">
         <v>63</v>
       </c>
@@ -20865,7 +21382,7 @@
         <v>32.4</v>
       </c>
     </row>
-    <row r="254" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A254">
         <v>64</v>
       </c>
@@ -20895,7 +21412,7 @@
         <v>39.205100000000002</v>
       </c>
     </row>
-    <row r="255" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A255">
         <v>64</v>
       </c>
@@ -20925,7 +21442,7 @@
         <v>56.903300000000016</v>
       </c>
     </row>
-    <row r="256" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A256">
         <v>64</v>
       </c>
@@ -27078,10 +27595,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10EE10AC-039B-7246-BB19-795F61BBEE1F}">
-  <dimension ref="A1:E73"/>
+  <dimension ref="A1:E120"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B73"/>
+    <sheetView topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="I115" sqref="I115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -28293,7 +28810,7 @@
         <v>105</v>
       </c>
       <c r="B68" s="5" t="str">
-        <f t="shared" ref="B68:B73" si="1">MID(A68,5,5)</f>
+        <f t="shared" ref="B68:B120" si="1">MID(A68,5,5)</f>
         <v>F3-39</v>
       </c>
       <c r="C68" s="6">
@@ -28394,6 +28911,852 @@
       </c>
       <c r="E73" s="8">
         <v>0.15494781506849878</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A74" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B74" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>F1-62</v>
+      </c>
+      <c r="C74" s="6">
+        <v>14.226351876830869</v>
+      </c>
+      <c r="D74" s="7">
+        <v>222.31040627747802</v>
+      </c>
+      <c r="E74" s="8">
+        <v>0.13316378071010068</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A75" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B75" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>F2-62</v>
+      </c>
+      <c r="C75" s="6">
+        <v>14.191341775350649</v>
+      </c>
+      <c r="D75" s="7">
+        <v>215.72683116526787</v>
+      </c>
+      <c r="E75" s="8">
+        <v>0.14608727899638632</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A76" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B76" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>F3-62</v>
+      </c>
+      <c r="C76" s="6">
+        <v>14.205443592326224</v>
+      </c>
+      <c r="D76" s="7">
+        <v>230.03500705713708</v>
+      </c>
+      <c r="E76" s="8">
+        <v>0.14186298530970723</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A77" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B77" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>F4-62</v>
+      </c>
+      <c r="C77" s="6">
+        <v>14.199060334152474</v>
+      </c>
+      <c r="D77" s="7">
+        <v>230.77163431382317</v>
+      </c>
+      <c r="E77" s="8">
+        <v>0.12255515900393749</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A78" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B78" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>F1-59</v>
+      </c>
+      <c r="C78" s="6">
+        <v>14.83243417635699</v>
+      </c>
+      <c r="D78" s="7">
+        <v>223.11333641621096</v>
+      </c>
+      <c r="E78" s="8">
+        <v>0.13357809354702721</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A79" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B79" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>F2-59</v>
+      </c>
+      <c r="C79" s="6">
+        <v>14.731503774128422</v>
+      </c>
+      <c r="D79" s="7">
+        <v>219.05562138639962</v>
+      </c>
+      <c r="E79" s="8">
+        <v>0.10422868399678681</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A80" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B80" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>F3-59</v>
+      </c>
+      <c r="C80" s="6">
+        <v>14.66241234508437</v>
+      </c>
+      <c r="D80" s="7">
+        <v>232.0577134677041</v>
+      </c>
+      <c r="E80" s="8">
+        <v>0.1153421798310512</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A81" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B81" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>F4-59</v>
+      </c>
+      <c r="C81" s="6">
+        <v>15.438007115511359</v>
+      </c>
+      <c r="D81" s="7">
+        <v>232.33512183528407</v>
+      </c>
+      <c r="E81" s="8">
+        <v>0.1072978023933663</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A82" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B82" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>F1-57</v>
+      </c>
+      <c r="C82" s="6">
+        <v>14.206518322564211</v>
+      </c>
+      <c r="D82" s="7">
+        <v>222.59276834506252</v>
+      </c>
+      <c r="E82" s="8">
+        <v>0.12147748257612119</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A83" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B83" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>F2-57</v>
+      </c>
+      <c r="C83" s="6">
+        <v>14.396573646771763</v>
+      </c>
+      <c r="D83" s="7">
+        <v>221.96672930627574</v>
+      </c>
+      <c r="E83" s="8">
+        <v>0.1249590480826368</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A84" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B84" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>F3-57</v>
+      </c>
+      <c r="C84" s="6">
+        <v>14.152129733484934</v>
+      </c>
+      <c r="D84" s="7">
+        <v>232.27201176317521</v>
+      </c>
+      <c r="E84" s="8">
+        <v>0.11791254751119029</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A85" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B85" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>F1-56</v>
+      </c>
+      <c r="C85" s="6">
+        <v>14.547797352410246</v>
+      </c>
+      <c r="D85" s="7">
+        <v>228.83649911025572</v>
+      </c>
+      <c r="E85" s="8">
+        <v>0.22233926079185029</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A86" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B86" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>F2-56</v>
+      </c>
+      <c r="C86" s="6">
+        <v>14.19029960478913</v>
+      </c>
+      <c r="D86" s="7">
+        <v>224.55323864462892</v>
+      </c>
+      <c r="E86" s="8">
+        <v>0.13788656173788003</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A87" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B87" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>F3-56</v>
+      </c>
+      <c r="C87" s="6">
+        <v>14.371108063794351</v>
+      </c>
+      <c r="D87" s="7">
+        <v>234.83967076096826</v>
+      </c>
+      <c r="E87" s="8">
+        <v>0.1508905558534247</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A88" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B88" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>F4-56</v>
+      </c>
+      <c r="C88" s="6">
+        <v>14.291224787671471</v>
+      </c>
+      <c r="D88" s="7">
+        <v>234.16530063745256</v>
+      </c>
+      <c r="E88" s="8">
+        <v>0.1571831809419327</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A89" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B89" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>F1-55</v>
+      </c>
+      <c r="C89" s="6">
+        <v>15.713144691566701</v>
+      </c>
+      <c r="D89" s="7">
+        <v>228.95397140920653</v>
+      </c>
+      <c r="E89" s="8">
+        <v>0.1814288516507708</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A90" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B90" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>F2-55</v>
+      </c>
+      <c r="C90" s="6">
+        <v>17.439259705141964</v>
+      </c>
+      <c r="D90" s="7">
+        <v>229.49386012837763</v>
+      </c>
+      <c r="E90" s="8">
+        <v>0.12562215141813121</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A91" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B91" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>F3-55</v>
+      </c>
+      <c r="C91" s="6">
+        <v>17.878681867224639</v>
+      </c>
+      <c r="D91" s="7">
+        <v>234.99070753853155</v>
+      </c>
+      <c r="E91" s="8">
+        <v>0.13772086442261722</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A92" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B92" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>F4-55</v>
+      </c>
+      <c r="C92" s="6">
+        <v>18.250014864258027</v>
+      </c>
+      <c r="D92" s="7">
+        <v>234.39657297524838</v>
+      </c>
+      <c r="E92" s="8">
+        <v>0.14111745151918231</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A93" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B93" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>F1-53</v>
+      </c>
+      <c r="C93" s="6">
+        <v>14.416437878733555</v>
+      </c>
+      <c r="D93" s="7">
+        <v>231.10276627067952</v>
+      </c>
+      <c r="E93" s="8">
+        <v>0.17729294465374082</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A94" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B94" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>F2-53</v>
+      </c>
+      <c r="C94" s="6">
+        <v>14.425360436677311</v>
+      </c>
+      <c r="D94" s="7">
+        <v>230.46329757256197</v>
+      </c>
+      <c r="E94" s="8">
+        <v>0.12893741850001922</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A95" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B95" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>F3-53</v>
+      </c>
+      <c r="C95" s="6">
+        <v>14.339845523227581</v>
+      </c>
+      <c r="D95" s="7">
+        <v>235.53384216024318</v>
+      </c>
+      <c r="E95" s="8">
+        <v>0.1547822248713408</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A96" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B96" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>F4-53</v>
+      </c>
+      <c r="C96" s="6">
+        <v>14.410413501381923</v>
+      </c>
+      <c r="D96" s="7">
+        <v>235.24889049085141</v>
+      </c>
+      <c r="E96" s="8">
+        <v>0.14385097245959519</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A97" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B97" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>F1-49</v>
+      </c>
+      <c r="C97" s="6">
+        <v>13.214068277703049</v>
+      </c>
+      <c r="D97" s="7">
+        <v>249.13725106757619</v>
+      </c>
+      <c r="E97" s="8">
+        <v>0.12379857720623</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A98" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B98" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>F2-49</v>
+      </c>
+      <c r="C98" s="6">
+        <v>13.220682766992441</v>
+      </c>
+      <c r="D98" s="7">
+        <v>247.55618257314066</v>
+      </c>
+      <c r="E98" s="8">
+        <v>0.12960042199727997</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A99" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B99" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>F3-49</v>
+      </c>
+      <c r="C99" s="6">
+        <v>13.223159121887248</v>
+      </c>
+      <c r="D99" s="7">
+        <v>248.26760189999709</v>
+      </c>
+      <c r="E99" s="8">
+        <v>0.16877092760610471</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A100" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B100" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>F4-49</v>
+      </c>
+      <c r="C100" s="6">
+        <v>13.185329208199558</v>
+      </c>
+      <c r="D100" s="7">
+        <v>249.29543370935659</v>
+      </c>
+      <c r="E100" s="8">
+        <v>0.12214067327007</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A101" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B101" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>F1-51</v>
+      </c>
+      <c r="C101" s="6">
+        <v>14.392600776679016</v>
+      </c>
+      <c r="D101" s="7">
+        <v>239.33028294095988</v>
+      </c>
+      <c r="E101" s="8">
+        <v>0.12844015495726682</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A102" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="B102" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>F2-51</v>
+      </c>
+      <c r="C102" s="6">
+        <v>14.47264281585552</v>
+      </c>
+      <c r="D102" s="7">
+        <v>237.29876576298457</v>
+      </c>
+      <c r="E102" s="8">
+        <v>0.1131861949266012</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A103" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B103" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>F3-51</v>
+      </c>
+      <c r="C103" s="6">
+        <v>14.472610252618576</v>
+      </c>
+      <c r="D103" s="7">
+        <v>240.31421891618737</v>
+      </c>
+      <c r="E103" s="8">
+        <v>0.12238936549037671</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A104" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B104" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>F4-51</v>
+      </c>
+      <c r="C104" s="6">
+        <v>14.423634543541228</v>
+      </c>
+      <c r="D104" s="7">
+        <v>241.16271620948774</v>
+      </c>
+      <c r="E104" s="8">
+        <v>0.10945426724932469</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A105" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B105" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>F1-52</v>
+      </c>
+      <c r="C105" s="6">
+        <v>14.47938339447602</v>
+      </c>
+      <c r="D105" s="7">
+        <v>237.11349162551934</v>
+      </c>
+      <c r="E105" s="8">
+        <v>0.14923435228718068</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A106" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B106" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>F2-52</v>
+      </c>
+      <c r="C106" s="6">
+        <v>14.571469794604063</v>
+      </c>
+      <c r="D106" s="7">
+        <v>233.15378503825872</v>
+      </c>
+      <c r="E106" s="8">
+        <v>0.14459642903148628</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A107" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B107" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>F3-52</v>
+      </c>
+      <c r="C107" s="6">
+        <v>14.485179622638841</v>
+      </c>
+      <c r="D107" s="7">
+        <v>239.51802476251896</v>
+      </c>
+      <c r="E107" s="8">
+        <v>0.12479326964880919</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A108" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B108" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>F4-52</v>
+      </c>
+      <c r="C108" s="6">
+        <v>14.445940783331913</v>
+      </c>
+      <c r="D108" s="7">
+        <v>237.06556263227267</v>
+      </c>
+      <c r="E108" s="8">
+        <v>0.14492773630355749</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A109" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="B109" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>F1-48</v>
+      </c>
+      <c r="C109" s="6">
+        <v>13.569395034472938</v>
+      </c>
+      <c r="D109" s="7">
+        <v>248.07309348138384</v>
+      </c>
+      <c r="E109" s="8">
+        <v>0.12255515900393749</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A110" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B110" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>F2-48</v>
+      </c>
+      <c r="C110" s="6">
+        <v>13.817981964522671</v>
+      </c>
+      <c r="D110" s="7">
+        <v>248.74082507842834</v>
+      </c>
+      <c r="E110" s="8">
+        <v>0.1168346818067228</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A111" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B111" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>F3-48</v>
+      </c>
+      <c r="C111" s="6">
+        <v>13.741399244920672</v>
+      </c>
+      <c r="D111" s="7">
+        <v>249.8373891970503</v>
+      </c>
+      <c r="E111" s="8">
+        <v>0.1459216331602127</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A112" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B112" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>F4-48</v>
+      </c>
+      <c r="C112" s="6">
+        <v>13.635918114559018</v>
+      </c>
+      <c r="D112" s="7">
+        <v>250.92342462093254</v>
+      </c>
+      <c r="E112" s="8">
+        <v>0.14376814265163029</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A113" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B113" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>F1-45</v>
+      </c>
+      <c r="C113" s="6">
+        <v>12.966612013782999</v>
+      </c>
+      <c r="D113" s="7">
+        <v>249.21736979897349</v>
+      </c>
+      <c r="E113" s="8">
+        <v>0.13763801537499271</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A114" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="B114" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>F2-45</v>
+      </c>
+      <c r="C114" s="6">
+        <v>13.024943281946751</v>
+      </c>
+      <c r="D114" s="7">
+        <v>249.57884596854538</v>
+      </c>
+      <c r="E114" s="8">
+        <v>0.1373894666721468</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A115" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B115" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>F3-45</v>
+      </c>
+      <c r="C115" s="6">
+        <v>12.970294429048135</v>
+      </c>
+      <c r="D115" s="7">
+        <v>250.22138710608178</v>
+      </c>
+      <c r="E115" s="8">
+        <v>0.1389635689375367</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A116" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B116" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>F4-45</v>
+      </c>
+      <c r="C116" s="6">
+        <v>13.116770848998399</v>
+      </c>
+      <c r="D116" s="7">
+        <v>252.46004013629351</v>
+      </c>
+      <c r="E116" s="8">
+        <v>0.21110557619715753</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A117" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="B117" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>F1-44</v>
+      </c>
+      <c r="C117" s="6">
+        <v>19.14984585958593</v>
+      </c>
+      <c r="D117" s="7">
+        <v>249.16154779304591</v>
+      </c>
+      <c r="E117" s="8">
+        <v>0.1398748484024688</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A118" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B118" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>F2-44</v>
+      </c>
+      <c r="C118" s="6">
+        <v>53.744562692455446</v>
+      </c>
+      <c r="D118" s="7">
+        <v>252.83993212089996</v>
+      </c>
+      <c r="E118" s="8">
+        <v>0.13722376623693922</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A119" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B119" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>F3-44</v>
+      </c>
+      <c r="C119" s="6">
+        <v>16.289495765805054</v>
+      </c>
+      <c r="D119" s="7">
+        <v>250.54300260120752</v>
+      </c>
+      <c r="E119" s="8">
+        <v>0.11326912067286871</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A120" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="B120" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>F4-44</v>
+      </c>
+      <c r="C120" s="6">
+        <v>15.197629372884938</v>
+      </c>
+      <c r="D120" s="7">
+        <v>251.33168362264513</v>
+      </c>
+      <c r="E120" s="8">
+        <v>0.18061977447124519</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding tracer injection modelling script
</commit_message>
<xml_diff>
--- a/data/exp_raw/no2_analyticall_results.xlsx
+++ b/data/exp_raw/no2_analyticall_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vcantarella/Documents/FuhrbergerColumns/data/exp_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{852CE026-617D-E24E-9EAA-356633E87A15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37683FF8-4EBD-EC49-BD5D-A62BB2709C87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="740" windowWidth="28040" windowHeight="16680" activeTab="6" xr2:uid="{3CD87C21-EA08-D841-BE93-D5199CA9A403}"/>
+    <workbookView xWindow="1080" yWindow="740" windowWidth="28040" windowHeight="16680" activeTab="6" xr2:uid="{3CD87C21-EA08-D841-BE93-D5199CA9A403}"/>
   </bookViews>
   <sheets>
     <sheet name="standard_curve_plate_1" sheetId="3" r:id="rId1"/>
@@ -7412,8 +7412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F829B9D-AC25-3345-89CA-34CFFCBEFC3A}">
   <dimension ref="A1:M221"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView topLeftCell="A198" workbookViewId="0">
+      <selection activeCell="L210" sqref="L210:L213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23721,8 +23721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28553D95-A703-174C-8A27-2C251D35502B}">
   <dimension ref="A1:P465"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B366" zoomScale="110" workbookViewId="0">
-      <selection activeCell="M254" sqref="M254:N257"/>
+    <sheetView tabSelected="1" topLeftCell="A357" zoomScale="110" workbookViewId="0">
+      <selection activeCell="P369" sqref="P369"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -36614,7 +36614,7 @@
         <v>2436.4166666666665</v>
       </c>
     </row>
-    <row r="369" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A369">
         <v>92</v>
       </c>
@@ -36651,8 +36651,12 @@
         <f>VLOOKUP(C369,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2491.5625</v>
       </c>
-    </row>
-    <row r="370" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P369">
+        <f>234/96*1000</f>
+        <v>2437.5</v>
+      </c>
+    </row>
+    <row r="370" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A370">
         <v>93</v>
       </c>
@@ -36683,7 +36687,7 @@
       </c>
       <c r="N370" s="12"/>
     </row>
-    <row r="371" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A371">
         <v>93</v>
       </c>
@@ -36714,7 +36718,7 @@
       </c>
       <c r="N371" s="12"/>
     </row>
-    <row r="372" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A372">
         <v>93</v>
       </c>
@@ -36745,7 +36749,7 @@
       </c>
       <c r="N372" s="12"/>
     </row>
-    <row r="373" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A373">
         <v>93</v>
       </c>
@@ -36776,7 +36780,7 @@
       </c>
       <c r="N373" s="12"/>
     </row>
-    <row r="374" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A374">
         <v>94</v>
       </c>
@@ -36803,7 +36807,7 @@
       </c>
       <c r="N374" s="12"/>
     </row>
-    <row r="375" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A375">
         <v>94</v>
       </c>
@@ -36830,7 +36834,7 @@
       </c>
       <c r="N375" s="12"/>
     </row>
-    <row r="376" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A376">
         <v>94</v>
       </c>
@@ -36857,7 +36861,7 @@
       </c>
       <c r="N376" s="12"/>
     </row>
-    <row r="377" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A377">
         <v>94</v>
       </c>
@@ -36884,7 +36888,7 @@
       </c>
       <c r="N377" s="12"/>
     </row>
-    <row r="378" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A378">
         <v>95</v>
       </c>
@@ -36922,7 +36926,7 @@
         <v>2422.2291666666665</v>
       </c>
     </row>
-    <row r="379" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A379">
         <v>95</v>
       </c>
@@ -36960,7 +36964,7 @@
         <v>2383.65625</v>
       </c>
     </row>
-    <row r="380" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A380">
         <v>95</v>
       </c>
@@ -36998,7 +37002,7 @@
         <v>2468.4791666666665</v>
       </c>
     </row>
-    <row r="381" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A381">
         <v>95</v>
       </c>
@@ -37036,7 +37040,7 @@
         <v>2510.2395833333335</v>
       </c>
     </row>
-    <row r="382" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A382">
         <v>96</v>
       </c>
@@ -37067,7 +37071,7 @@
       </c>
       <c r="N382" s="12"/>
     </row>
-    <row r="383" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A383">
         <v>96</v>
       </c>
@@ -37098,7 +37102,7 @@
       </c>
       <c r="N383" s="12"/>
     </row>
-    <row r="384" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A384">
         <v>96</v>
       </c>

</xml_diff>

<commit_message>
error analysis and new data for the new experiment
</commit_message>
<xml_diff>
--- a/data/exp_raw/no2_analyticall_results.xlsx
+++ b/data/exp_raw/no2_analyticall_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vcantarella/Documents/FuhrbergerColumns/data/exp_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37683FF8-4EBD-EC49-BD5D-A62BB2709C87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{321BD3B8-8A76-C443-9FEB-EBAC4153D36B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="740" windowWidth="28040" windowHeight="16680" activeTab="6" xr2:uid="{3CD87C21-EA08-D841-BE93-D5199CA9A403}"/>
+    <workbookView xWindow="1080" yWindow="740" windowWidth="28040" windowHeight="16680" xr2:uid="{3CD87C21-EA08-D841-BE93-D5199CA9A403}"/>
   </bookViews>
   <sheets>
     <sheet name="standard_curve_plate_1" sheetId="3" r:id="rId1"/>
@@ -1317,7 +1317,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -1366,7 +1366,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1380,8 +1380,7 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6894,8 +6893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8016D5F0-D8DF-6146-A719-90B0660FC49C}">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22264,7 +22263,7 @@
         <v>45825.369444444441</v>
       </c>
       <c r="E3" s="11">
-        <f t="shared" ref="E3:E53" si="0">C3+(D3-C3)/2</f>
+        <f t="shared" ref="E3:E5" si="0">C3+(D3-C3)/2</f>
         <v>45825.159722222219</v>
       </c>
       <c r="F3">
@@ -23721,7 +23720,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28553D95-A703-174C-8A27-2C251D35502B}">
   <dimension ref="A1:P465"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A357" zoomScale="110" workbookViewId="0">
+    <sheetView topLeftCell="A196" zoomScale="110" workbookViewId="0">
       <selection activeCell="P369" sqref="P369"/>
     </sheetView>
   </sheetViews>
@@ -32436,7 +32435,7 @@
         <f>VLOOKUP(C250,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>1.6290322580645162</v>
       </c>
-      <c r="N250" s="12">
+      <c r="N250">
         <f>VLOOKUP(C250,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2302.1979166666665</v>
       </c>
@@ -32473,7 +32472,7 @@
         <f>VLOOKUP(C251,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>1.5806451612903225</v>
       </c>
-      <c r="N251" s="12">
+      <c r="N251">
         <f>VLOOKUP(C251,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2257.4479166666665</v>
       </c>
@@ -32510,7 +32509,7 @@
         <f>VLOOKUP(C252,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>1.774193548387097</v>
       </c>
-      <c r="N252" s="12">
+      <c r="N252">
         <f>VLOOKUP(C252,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2392.770833333333</v>
       </c>
@@ -32547,7 +32546,7 @@
         <f>VLOOKUP(C253,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>1.8225806451612903</v>
       </c>
-      <c r="N253" s="12">
+      <c r="N253">
         <f>VLOOKUP(C253,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2390.125</v>
       </c>
@@ -32581,7 +32580,6 @@
         <f>VLOOKUP(sampling!C254,fe_plate_1!$C$2:$G$80,5,FALSE)</f>
         <v>39.205100000000002</v>
       </c>
-      <c r="N254" s="12"/>
     </row>
     <row r="255" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A255">
@@ -32612,7 +32610,6 @@
         <f>VLOOKUP(sampling!C255,fe_plate_1!$C$2:$G$80,5,FALSE)</f>
         <v>56.903300000000016</v>
       </c>
-      <c r="N255" s="12"/>
     </row>
     <row r="256" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A256">
@@ -32643,7 +32640,6 @@
         <f>VLOOKUP(sampling!C256,fe_plate_1!$C$2:$G$80,5,FALSE)</f>
         <v>26.952500000000011</v>
       </c>
-      <c r="N256" s="12"/>
     </row>
     <row r="257" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A257">
@@ -32674,7 +32670,6 @@
         <f>VLOOKUP(sampling!C257,fe_plate_1!$C$2:$G$80,5,FALSE)</f>
         <v>12.657800000000005</v>
       </c>
-      <c r="N257" s="12"/>
     </row>
     <row r="258" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A258">
@@ -32708,7 +32703,7 @@
         <f>VLOOKUP(C258,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>1.5</v>
       </c>
-      <c r="N258" s="12">
+      <c r="N258">
         <f>VLOOKUP(C258,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2341.8125</v>
       </c>
@@ -32745,7 +32740,7 @@
         <f>VLOOKUP(C259,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>1.7419354838709677</v>
       </c>
-      <c r="N259" s="12">
+      <c r="N259">
         <f>VLOOKUP(C259,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2247.0416666666665</v>
       </c>
@@ -32782,7 +32777,7 @@
         <f>VLOOKUP(C260,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>1.6290322580645162</v>
       </c>
-      <c r="N260" s="12">
+      <c r="N260">
         <f>VLOOKUP(C260,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2396.34375</v>
       </c>
@@ -32819,7 +32814,7 @@
         <f>VLOOKUP(C261,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>1.9677419354838708</v>
       </c>
-      <c r="N261" s="12">
+      <c r="N261">
         <f>VLOOKUP(C261,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2422.0937499999995</v>
       </c>
@@ -32852,7 +32847,6 @@
       <c r="H262">
         <v>30.7</v>
       </c>
-      <c r="N262" s="12"/>
     </row>
     <row r="263" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A263">
@@ -32882,7 +32876,6 @@
       <c r="H263">
         <v>31.8</v>
       </c>
-      <c r="N263" s="12"/>
     </row>
     <row r="264" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A264">
@@ -32912,7 +32905,6 @@
       <c r="H264">
         <v>30.5</v>
       </c>
-      <c r="N264" s="12"/>
     </row>
     <row r="265" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A265">
@@ -32942,7 +32934,6 @@
       <c r="H265">
         <v>31.4</v>
       </c>
-      <c r="N265" s="12"/>
     </row>
     <row r="266" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A266">
@@ -32982,7 +32973,7 @@
         <f>VLOOKUP(C266,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>0.25806451612903225</v>
       </c>
-      <c r="N266" s="12">
+      <c r="N266">
         <f>VLOOKUP(C266,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2274.135416666667</v>
       </c>
@@ -33025,7 +33016,7 @@
         <f>VLOOKUP(C267,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>0.35483870967741932</v>
       </c>
-      <c r="N267" s="12">
+      <c r="N267">
         <f>VLOOKUP(C267,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2248.0625</v>
       </c>
@@ -33068,7 +33059,7 @@
         <f>VLOOKUP(C268,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>0.29032258064516125</v>
       </c>
-      <c r="N268" s="12">
+      <c r="N268">
         <f>VLOOKUP(C268,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2313.6041666666665</v>
       </c>
@@ -33111,7 +33102,7 @@
         <f>VLOOKUP(C269,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>0.54838709677419362</v>
       </c>
-      <c r="N269" s="12">
+      <c r="N269">
         <f>VLOOKUP(C269,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2349.3749999999995</v>
       </c>
@@ -33145,7 +33136,6 @@
         <f>VLOOKUP(sampling!C270,fe_plate_1!$C$2:$G$80,5,FALSE)</f>
         <v>34.440200000000004</v>
       </c>
-      <c r="N270" s="12"/>
     </row>
     <row r="271" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A271">
@@ -33176,7 +33166,6 @@
         <f>VLOOKUP(sampling!C271,fe_plate_1!$C$2:$G$80,5,FALSE)</f>
         <v>59.626100000000008</v>
       </c>
-      <c r="N271" s="12"/>
     </row>
     <row r="272" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A272">
@@ -33207,7 +33196,6 @@
         <f>VLOOKUP(sampling!C272,fe_plate_1!$C$2:$G$80,5,FALSE)</f>
         <v>33.759500000000003</v>
       </c>
-      <c r="N272" s="12"/>
     </row>
     <row r="273" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A273">
@@ -33238,7 +33226,6 @@
         <f>VLOOKUP(sampling!C273,fe_plate_1!$C$2:$G$80,5,FALSE)</f>
         <v>18.784099999999999</v>
       </c>
-      <c r="N273" s="12"/>
     </row>
     <row r="274" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A274">
@@ -33265,7 +33252,6 @@
         <f t="shared" si="13"/>
         <v>16.251736111109494</v>
       </c>
-      <c r="N274" s="12"/>
     </row>
     <row r="275" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A275">
@@ -33292,7 +33278,6 @@
         <f t="shared" si="13"/>
         <v>16.251736111109494</v>
       </c>
-      <c r="N275" s="12"/>
     </row>
     <row r="276" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A276">
@@ -33326,7 +33311,7 @@
         <f>VLOOKUP(C276,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>0</v>
       </c>
-      <c r="N276" s="12">
+      <c r="N276">
         <f>VLOOKUP(C276,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2310.041666666667</v>
       </c>
@@ -33363,7 +33348,7 @@
         <f>VLOOKUP(C277,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>0</v>
       </c>
-      <c r="N277" s="12">
+      <c r="N277">
         <f>VLOOKUP(C277,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2367.6666666666665</v>
       </c>
@@ -33410,7 +33395,7 @@
         <f>VLOOKUP(C278,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>0.22580645161290325</v>
       </c>
-      <c r="N278" s="12">
+      <c r="N278">
         <f>VLOOKUP(C278,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2263.708333333333</v>
       </c>
@@ -33457,7 +33442,7 @@
         <f>VLOOKUP(C279,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>0</v>
       </c>
-      <c r="N279" s="12">
+      <c r="N279">
         <f>VLOOKUP(C279,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2214.21875</v>
       </c>
@@ -33504,7 +33489,7 @@
         <f>VLOOKUP(C280,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>0</v>
       </c>
-      <c r="N280" s="12">
+      <c r="N280">
         <f>VLOOKUP(C280,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2320.1666666666665</v>
       </c>
@@ -33551,7 +33536,7 @@
         <f>VLOOKUP(C281,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>0</v>
       </c>
-      <c r="N281" s="12">
+      <c r="N281">
         <f>VLOOKUP(C281,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2310.28125</v>
       </c>
@@ -33581,7 +33566,6 @@
         <f t="shared" si="13"/>
         <v>16.752777777779556</v>
       </c>
-      <c r="N282" s="12"/>
     </row>
     <row r="283" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A283">
@@ -33608,7 +33592,6 @@
         <f t="shared" si="13"/>
         <v>16.752777777779556</v>
       </c>
-      <c r="N283" s="12"/>
     </row>
     <row r="284" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A284">
@@ -33635,7 +33618,6 @@
         <f t="shared" si="13"/>
         <v>16.743055555562023</v>
       </c>
-      <c r="N284" s="12"/>
     </row>
     <row r="285" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A285">
@@ -33662,7 +33644,6 @@
         <f t="shared" si="13"/>
         <v>16.743055555562023</v>
       </c>
-      <c r="N285" s="12"/>
     </row>
     <row r="286" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A286">
@@ -33696,7 +33677,7 @@
         <f>VLOOKUP(C286,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>0</v>
       </c>
-      <c r="N286" s="12">
+      <c r="N286">
         <f>VLOOKUP(C286,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2197.21875</v>
       </c>
@@ -33733,7 +33714,7 @@
         <f>VLOOKUP(C287,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>0.33870967741935487</v>
       </c>
-      <c r="N287" s="12">
+      <c r="N287">
         <f>VLOOKUP(C287,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2241.9687500000005</v>
       </c>
@@ -33770,7 +33751,7 @@
         <f>VLOOKUP(C288,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>0.38709677419354838</v>
       </c>
-      <c r="N288" s="12">
+      <c r="N288">
         <f>VLOOKUP(C288,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2259.729166666667</v>
       </c>
@@ -33807,7 +33788,7 @@
         <f>VLOOKUP(C289,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>0.5161290322580645</v>
       </c>
-      <c r="N289" s="12">
+      <c r="N289">
         <f>VLOOKUP(C289,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2246.5520833333335</v>
       </c>
@@ -33848,7 +33829,7 @@
         <f>VLOOKUP(C290,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>0.33870967741935487</v>
       </c>
-      <c r="N290" s="12">
+      <c r="N290">
         <f>VLOOKUP(C290,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2241.8958333333335</v>
       </c>
@@ -33889,7 +33870,7 @@
         <f>VLOOKUP(C291,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>0.37096774193548387</v>
       </c>
-      <c r="N291" s="12">
+      <c r="N291">
         <f>VLOOKUP(C291,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2247.40625</v>
       </c>
@@ -33930,7 +33911,7 @@
         <f>VLOOKUP(C292,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>0.32258064516129031</v>
       </c>
-      <c r="N292" s="12">
+      <c r="N292">
         <f>VLOOKUP(C292,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2276.9895833333335</v>
       </c>
@@ -33971,7 +33952,7 @@
         <f>VLOOKUP(C293,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>0.32258064516129031</v>
       </c>
-      <c r="N293" s="12">
+      <c r="N293">
         <f>VLOOKUP(C293,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2253.5833333333335</v>
       </c>
@@ -34005,7 +33986,6 @@
         <f>VLOOKUP(sampling!C294,fe_plate_1!$C$2:$G$80,5,FALSE)</f>
         <v>37.843700000000013</v>
       </c>
-      <c r="N294" s="12"/>
     </row>
     <row r="295" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A295">
@@ -34036,7 +34016,6 @@
         <f>VLOOKUP(sampling!C295,fe_plate_1!$C$2:$G$80,5,FALSE)</f>
         <v>65.752399999999994</v>
       </c>
-      <c r="N295" s="12"/>
     </row>
     <row r="296" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A296">
@@ -34067,7 +34046,6 @@
         <f>VLOOKUP(sampling!C296,fe_plate_1!$C$2:$G$80,5,FALSE)</f>
         <v>34.440200000000004</v>
       </c>
-      <c r="N296" s="12"/>
     </row>
     <row r="297" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A297">
@@ -34098,7 +34076,6 @@
         <f>VLOOKUP(sampling!C297,fe_plate_1!$C$2:$G$80,5,FALSE)</f>
         <v>19.4648</v>
       </c>
-      <c r="N297" s="12"/>
     </row>
     <row r="298" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A298">
@@ -34129,7 +34106,6 @@
         <f>VLOOKUP(sampling!C298,fe_plate_1!$C$2:$G$80,5,FALSE)</f>
         <v>38.5244</v>
       </c>
-      <c r="N298" s="12"/>
     </row>
     <row r="299" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A299">
@@ -34160,7 +34136,6 @@
         <f>VLOOKUP(sampling!C299,fe_plate_1!$C$2:$G$80,5,FALSE)</f>
         <v>80.727800000000016</v>
       </c>
-      <c r="N299" s="12"/>
     </row>
     <row r="300" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A300">
@@ -34191,7 +34166,6 @@
         <f>VLOOKUP(sampling!C300,fe_plate_1!$C$2:$G$80,5,FALSE)</f>
         <v>31.717400000000001</v>
       </c>
-      <c r="N300" s="12"/>
     </row>
     <row r="301" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A301">
@@ -34222,7 +34196,6 @@
         <f>VLOOKUP(sampling!C301,fe_plate_1!$C$2:$G$80,5,FALSE)</f>
         <v>20.145500000000002</v>
       </c>
-      <c r="N301" s="12"/>
     </row>
     <row r="302" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A302">
@@ -34266,7 +34239,7 @@
         <f>VLOOKUP(C302,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>0.24193548387096775</v>
       </c>
-      <c r="N302" s="12">
+      <c r="N302">
         <f>VLOOKUP(C302,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2267.5520833333335</v>
       </c>
@@ -34313,7 +34286,7 @@
         <f>VLOOKUP(C303,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>0.24193548387096775</v>
       </c>
-      <c r="N303" s="12">
+      <c r="N303">
         <f>VLOOKUP(C303,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2267.96875</v>
       </c>
@@ -34360,7 +34333,7 @@
         <f>VLOOKUP(C304,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>0.59677419354838701</v>
       </c>
-      <c r="N304" s="12">
+      <c r="N304">
         <f>VLOOKUP(C304,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2313.0416666666665</v>
       </c>
@@ -34407,7 +34380,7 @@
         <f>VLOOKUP(C305,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>0.37096774193548387</v>
       </c>
-      <c r="N305" s="12">
+      <c r="N305">
         <f>VLOOKUP(C305,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2247.291666666667</v>
       </c>
@@ -34448,7 +34421,7 @@
         <f>VLOOKUP(C306,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>0.72580645161290314</v>
       </c>
-      <c r="N306" s="12">
+      <c r="N306">
         <f>VLOOKUP(C306,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2246.6041666666665</v>
       </c>
@@ -34489,7 +34462,7 @@
         <f>VLOOKUP(C307,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>0.19354838709677419</v>
       </c>
-      <c r="N307" s="12">
+      <c r="N307">
         <f>VLOOKUP(C307,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2252.291666666667</v>
       </c>
@@ -34530,7 +34503,7 @@
         <f>VLOOKUP(C308,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>0.56451612903225812</v>
       </c>
-      <c r="N308" s="12">
+      <c r="N308">
         <f>VLOOKUP(C308,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2355.78125</v>
       </c>
@@ -34571,7 +34544,7 @@
         <f>VLOOKUP(C309,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>1.5</v>
       </c>
-      <c r="N309" s="12">
+      <c r="N309">
         <f>VLOOKUP(C309,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2284.125</v>
       </c>
@@ -34604,7 +34577,6 @@
       <c r="H310">
         <v>32.299999999999997</v>
       </c>
-      <c r="N310" s="12"/>
     </row>
     <row r="311" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A311">
@@ -34634,7 +34606,6 @@
       <c r="H311">
         <v>32.799999999999997</v>
       </c>
-      <c r="N311" s="12"/>
     </row>
     <row r="312" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A312">
@@ -34664,7 +34635,6 @@
       <c r="H312">
         <v>34</v>
       </c>
-      <c r="N312" s="12"/>
     </row>
     <row r="313" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A313">
@@ -34694,7 +34664,6 @@
       <c r="H313">
         <v>30.9</v>
       </c>
-      <c r="N313" s="12"/>
     </row>
     <row r="314" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A314">
@@ -34729,7 +34698,7 @@
         <f>VLOOKUP(C314,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>0.32258064516129031</v>
       </c>
-      <c r="N314" s="12">
+      <c r="N314">
         <f>VLOOKUP(C314,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2243.9791666666665</v>
       </c>
@@ -34767,7 +34736,7 @@
         <f>VLOOKUP(C315,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>0.38709677419354838</v>
       </c>
-      <c r="N315" s="12">
+      <c r="N315">
         <f>VLOOKUP(C315,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2225.4166666666665</v>
       </c>
@@ -34805,7 +34774,7 @@
         <f>VLOOKUP(C316,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>0.37096774193548387</v>
       </c>
-      <c r="N316" s="12">
+      <c r="N316">
         <f>VLOOKUP(C316,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2344.916666666667</v>
       </c>
@@ -34843,7 +34812,7 @@
         <f>VLOOKUP(C317,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>0.967741935483871</v>
       </c>
-      <c r="N317" s="12">
+      <c r="N317">
         <f>VLOOKUP(C317,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2298.458333333333</v>
       </c>
@@ -34877,7 +34846,6 @@
         <f>VLOOKUP(sampling!C318,fe_plate_1!$C$2:$G$80,5,FALSE)</f>
         <v>46.012100000000004</v>
       </c>
-      <c r="N318" s="12"/>
     </row>
     <row r="319" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A319">
@@ -34908,7 +34876,6 @@
         <f>VLOOKUP(sampling!C319,fe_plate_1!$C$2:$G$80,5,FALSE)</f>
         <v>71.198000000000008</v>
       </c>
-      <c r="N319" s="12"/>
     </row>
     <row r="320" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A320">
@@ -34939,7 +34906,6 @@
         <f>VLOOKUP(sampling!C320,fe_plate_1!$C$2:$G$80,5,FALSE)</f>
         <v>37.843700000000013</v>
       </c>
-      <c r="N320" s="12"/>
     </row>
     <row r="321" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A321">
@@ -34970,7 +34936,6 @@
         <f>VLOOKUP(sampling!C321,fe_plate_1!$C$2:$G$80,5,FALSE)</f>
         <v>25.591100000000008</v>
       </c>
-      <c r="N321" s="12"/>
     </row>
     <row r="322" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A322">
@@ -34997,7 +34962,6 @@
         <f t="shared" si="13"/>
         <v>21.597916666658421</v>
       </c>
-      <c r="N322" s="12"/>
     </row>
     <row r="323" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A323">
@@ -35024,7 +34988,6 @@
         <f t="shared" si="13"/>
         <v>21.597916666658421</v>
       </c>
-      <c r="N323" s="12"/>
     </row>
     <row r="324" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A324">
@@ -35051,7 +35014,6 @@
         <f t="shared" ref="G324:G387" si="17" xml:space="preserve"> F324-IF(OR(B324=1,B324=2),$O$2,$O$3)</f>
         <v>21.588194444440887</v>
       </c>
-      <c r="N324" s="12"/>
     </row>
     <row r="325" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A325">
@@ -35078,7 +35040,6 @@
         <f t="shared" si="17"/>
         <v>21.588194444440887</v>
       </c>
-      <c r="N325" s="12"/>
     </row>
     <row r="326" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A326">
@@ -35113,7 +35074,7 @@
         <f>VLOOKUP(C326,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>2.532258064516129</v>
       </c>
-      <c r="N326" s="12">
+      <c r="N326">
         <f>VLOOKUP(C326,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2190.6041666666665</v>
       </c>
@@ -35151,7 +35112,7 @@
         <f>VLOOKUP(C327,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>0.45161290322580649</v>
       </c>
-      <c r="N327" s="12">
+      <c r="N327">
         <f>VLOOKUP(C327,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2229.3229166666665</v>
       </c>
@@ -35189,7 +35150,7 @@
         <f>VLOOKUP(C328,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>0.74193548387096775</v>
       </c>
-      <c r="N328" s="12">
+      <c r="N328">
         <f>VLOOKUP(C328,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2293.9374999999995</v>
       </c>
@@ -35227,7 +35188,7 @@
         <f>VLOOKUP(C329,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>0.41935483870967738</v>
       </c>
-      <c r="N329" s="12">
+      <c r="N329">
         <f>VLOOKUP(C329,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2300.7500000000005</v>
       </c>
@@ -35265,7 +35226,7 @@
         <f>VLOOKUP(C330,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>0.467741935483871</v>
       </c>
-      <c r="N330" s="12">
+      <c r="N330">
         <f>VLOOKUP(C330,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2252.84375</v>
       </c>
@@ -35303,7 +35264,7 @@
         <f>VLOOKUP(C331,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>118.66129032258064</v>
       </c>
-      <c r="N331" s="12">
+      <c r="N331">
         <f>VLOOKUP(C331,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2333.291666666667</v>
       </c>
@@ -35341,7 +35302,7 @@
         <f>VLOOKUP(C332,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>10.85483870967742</v>
       </c>
-      <c r="N332" s="12">
+      <c r="N332">
         <f>VLOOKUP(C332,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2380.864583333333</v>
       </c>
@@ -35379,7 +35340,7 @@
         <f>VLOOKUP(C333,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>16.258064516129032</v>
       </c>
-      <c r="N333" s="12">
+      <c r="N333">
         <f>VLOOKUP(C333,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2351.0625</v>
       </c>
@@ -35417,7 +35378,7 @@
         <f>VLOOKUP(C334,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>127.59677419354837</v>
       </c>
-      <c r="N334" s="12">
+      <c r="N334">
         <f>VLOOKUP(C334,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2370.1250000000005</v>
       </c>
@@ -35455,7 +35416,7 @@
         <f>VLOOKUP(C335,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>632.41935483870975</v>
       </c>
-      <c r="N335" s="12">
+      <c r="N335">
         <f>VLOOKUP(C335,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2408.2291666666665</v>
       </c>
@@ -35493,7 +35454,7 @@
         <f>VLOOKUP(C336,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>530.98387096774195</v>
       </c>
-      <c r="N336" s="12">
+      <c r="N336">
         <f>VLOOKUP(C336,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2403.1979166666665</v>
       </c>
@@ -35531,7 +35492,7 @@
         <f>VLOOKUP(C337,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>475.12903225806446</v>
       </c>
-      <c r="N337" s="12">
+      <c r="N337">
         <f>VLOOKUP(C337,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2472.8854166666665</v>
       </c>
@@ -35565,7 +35526,6 @@
         <f>VLOOKUP(sampling!C338,fe_plate_1!$C$2:$G$300,5,FALSE)</f>
         <v>13.338500000000007</v>
       </c>
-      <c r="N338" s="12"/>
     </row>
     <row r="339" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A339">
@@ -35596,7 +35556,6 @@
         <f>VLOOKUP(sampling!C339,fe_plate_1!$C$2:$G$300,5,FALSE)</f>
         <v>7.2122000000000064</v>
       </c>
-      <c r="N339" s="12"/>
     </row>
     <row r="340" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A340">
@@ -35627,7 +35586,6 @@
         <f>VLOOKUP(sampling!C340,fe_plate_1!$C$2:$G$300,5,FALSE)</f>
         <v>10.6157</v>
       </c>
-      <c r="N340" s="12"/>
     </row>
     <row r="341" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A341">
@@ -35658,7 +35616,6 @@
         <f>VLOOKUP(sampling!C341,fe_plate_1!$C$2:$G$300,5,FALSE)</f>
         <v>7.8929000000000009</v>
       </c>
-      <c r="N341" s="12"/>
     </row>
     <row r="342" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A342">
@@ -35693,7 +35650,7 @@
         <f>VLOOKUP(C342,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>151.67741935483872</v>
       </c>
-      <c r="N342" s="12">
+      <c r="N342">
         <f>VLOOKUP(C342,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2516.875</v>
       </c>
@@ -35731,7 +35688,7 @@
         <f>VLOOKUP(C343,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>68.967741935483872</v>
       </c>
-      <c r="N343" s="12">
+      <c r="N343">
         <f>VLOOKUP(C343,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2482.46875</v>
       </c>
@@ -35769,7 +35726,7 @@
         <f>VLOOKUP(C344,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>757.0645161290322</v>
       </c>
-      <c r="N344" s="12">
+      <c r="N344">
         <f>VLOOKUP(C344,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2456.4583333333335</v>
       </c>
@@ -35807,7 +35764,7 @@
         <f>VLOOKUP(C345,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>266.96774193548384</v>
       </c>
-      <c r="N345" s="12">
+      <c r="N345">
         <f>VLOOKUP(C345,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2483.552083333333</v>
       </c>
@@ -35841,7 +35798,7 @@
         <f>VLOOKUP(C346,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>13.5</v>
       </c>
-      <c r="N346" s="12">
+      <c r="N346">
         <f>VLOOKUP(C346,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2481.895833333333</v>
       </c>
@@ -35875,7 +35832,7 @@
         <f>VLOOKUP(C347,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>2.5483870967741939</v>
       </c>
-      <c r="N347" s="12">
+      <c r="N347">
         <f>VLOOKUP(C347,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2460.9479166666665</v>
       </c>
@@ -35909,7 +35866,7 @@
         <f>VLOOKUP(C348,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>192.08064516129033</v>
       </c>
-      <c r="N348" s="12">
+      <c r="N348">
         <f>VLOOKUP(C348,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2457.333333333333</v>
       </c>
@@ -35943,7 +35900,7 @@
         <f>VLOOKUP(C349,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>3.1290322580645165</v>
       </c>
-      <c r="N349" s="12">
+      <c r="N349">
         <f>VLOOKUP(C349,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2472.1354166666665</v>
       </c>
@@ -35977,7 +35934,6 @@
         <f>VLOOKUP(sampling!C350,fe_plate_1!$C$2:$G$300,5,FALSE)</f>
         <v>9.2542999999999971</v>
       </c>
-      <c r="N350" s="12"/>
     </row>
     <row r="351" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A351">
@@ -36008,7 +35964,6 @@
         <f>VLOOKUP(sampling!C351,fe_plate_1!$C$2:$G$300,5,FALSE)</f>
         <v>11.977100000000004</v>
       </c>
-      <c r="N351" s="12"/>
     </row>
     <row r="352" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A352">
@@ -36039,7 +35994,6 @@
         <f>VLOOKUP(sampling!C352,fe_plate_1!$C$2:$G$300,5,FALSE)</f>
         <v>11.296400000000002</v>
       </c>
-      <c r="N352" s="12"/>
     </row>
     <row r="353" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A353">
@@ -36070,7 +36024,6 @@
         <f>VLOOKUP(sampling!C353,fe_plate_1!$C$2:$G$300,5,FALSE)</f>
         <v>9.2542999999999971</v>
       </c>
-      <c r="N353" s="12"/>
     </row>
     <row r="354" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A354">
@@ -36105,7 +36058,7 @@
         <f>VLOOKUP(C354,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>0.74193548387096775</v>
       </c>
-      <c r="N354" s="12">
+      <c r="N354">
         <f>VLOOKUP(C354,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2420.166666666667</v>
       </c>
@@ -36143,7 +36096,7 @@
         <f>VLOOKUP(C355,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>0.90322580645161299</v>
       </c>
-      <c r="N355" s="12">
+      <c r="N355">
         <f>VLOOKUP(C355,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2410.458333333333</v>
       </c>
@@ -36181,7 +36134,7 @@
         <f>VLOOKUP(C356,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>0.35483870967741932</v>
       </c>
-      <c r="N356" s="12">
+      <c r="N356">
         <f>VLOOKUP(C356,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2472.6041666666665</v>
       </c>
@@ -36219,7 +36172,7 @@
         <f>VLOOKUP(C357,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>0.41935483870967738</v>
       </c>
-      <c r="N357" s="12">
+      <c r="N357">
         <f>VLOOKUP(C357,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2470.4166666666665</v>
       </c>
@@ -36253,7 +36206,6 @@
         <f>VLOOKUP(sampling!C358,fe_plate_1!$C$2:$G$300,5,FALSE)</f>
         <v>26.27180000000001</v>
       </c>
-      <c r="N358" s="12"/>
     </row>
     <row r="359" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A359">
@@ -36284,7 +36236,6 @@
         <f>VLOOKUP(sampling!C359,fe_plate_1!$C$2:$G$300,5,FALSE)</f>
         <v>28.3139</v>
       </c>
-      <c r="N359" s="12"/>
     </row>
     <row r="360" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A360">
@@ -36315,7 +36266,6 @@
         <f>VLOOKUP(sampling!C360,fe_plate_1!$C$2:$G$300,5,FALSE)</f>
         <v>14.019200000000009</v>
       </c>
-      <c r="N360" s="12"/>
     </row>
     <row r="361" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A361">
@@ -36346,7 +36296,6 @@
         <f>VLOOKUP(sampling!C361,fe_plate_1!$C$2:$G$300,5,FALSE)</f>
         <v>18.103399999999997</v>
       </c>
-      <c r="N361" s="12"/>
     </row>
     <row r="362" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A362">
@@ -36381,7 +36330,7 @@
         <f>VLOOKUP(C362,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>0.74193548387096775</v>
       </c>
-      <c r="N362" s="12">
+      <c r="N362">
         <f>VLOOKUP(C362,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2452.5520833333335</v>
       </c>
@@ -36419,7 +36368,7 @@
         <f>VLOOKUP(C363,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>0.98387096774193539</v>
       </c>
-      <c r="N363" s="12">
+      <c r="N363">
         <f>VLOOKUP(C363,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2420.46875</v>
       </c>
@@ -36457,7 +36406,7 @@
         <f>VLOOKUP(C364,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>0.75806451612903225</v>
       </c>
-      <c r="N364" s="12">
+      <c r="N364">
         <f>VLOOKUP(C364,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2480.6145833333335</v>
       </c>
@@ -36495,7 +36444,7 @@
         <f>VLOOKUP(C365,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>0.59677419354838701</v>
       </c>
-      <c r="N365" s="12">
+      <c r="N365">
         <f>VLOOKUP(C365,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2444.520833333333</v>
       </c>
@@ -36533,7 +36482,7 @@
         <f>VLOOKUP(C366,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>0.70967741935483863</v>
       </c>
-      <c r="N366" s="12">
+      <c r="N366">
         <f>VLOOKUP(C366,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2440.875</v>
       </c>
@@ -36571,7 +36520,7 @@
         <f>VLOOKUP(C367,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>1</v>
       </c>
-      <c r="N367" s="12">
+      <c r="N367">
         <f>VLOOKUP(C367,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2405.6041666666665</v>
       </c>
@@ -36609,7 +36558,7 @@
         <f>VLOOKUP(C368,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>0.43548387096774194</v>
       </c>
-      <c r="N368" s="12">
+      <c r="N368">
         <f>VLOOKUP(C368,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2436.4166666666665</v>
       </c>
@@ -36647,7 +36596,7 @@
         <f>VLOOKUP(C369,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>0.56451612903225812</v>
       </c>
-      <c r="N369" s="12">
+      <c r="N369">
         <f>VLOOKUP(C369,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2491.5625</v>
       </c>
@@ -36685,7 +36634,6 @@
         <f>VLOOKUP(sampling!C370,fe_plate_1!$C$2:$G$300,5,FALSE)</f>
         <v>18.103399999999997</v>
       </c>
-      <c r="N370" s="12"/>
     </row>
     <row r="371" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A371">
@@ -36716,7 +36664,6 @@
         <f>VLOOKUP(sampling!C371,fe_plate_1!$C$2:$G$300,5,FALSE)</f>
         <v>26.27180000000001</v>
       </c>
-      <c r="N371" s="12"/>
     </row>
     <row r="372" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A372">
@@ -36747,7 +36694,6 @@
         <f>VLOOKUP(sampling!C372,fe_plate_1!$C$2:$G$300,5,FALSE)</f>
         <v>36.482300000000009</v>
       </c>
-      <c r="N372" s="12"/>
     </row>
     <row r="373" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A373">
@@ -36778,7 +36724,6 @@
         <f>VLOOKUP(sampling!C373,fe_plate_1!$C$2:$G$300,5,FALSE)</f>
         <v>19.4648</v>
       </c>
-      <c r="N373" s="12"/>
     </row>
     <row r="374" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A374">
@@ -36805,7 +36750,6 @@
         <f t="shared" si="17"/>
         <v>26.152777777773736</v>
       </c>
-      <c r="N374" s="12"/>
     </row>
     <row r="375" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A375">
@@ -36832,7 +36776,6 @@
         <f t="shared" si="17"/>
         <v>26.152777777773736</v>
       </c>
-      <c r="N375" s="12"/>
     </row>
     <row r="376" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A376">
@@ -36859,7 +36802,6 @@
         <f t="shared" si="17"/>
         <v>26.143055555556202</v>
       </c>
-      <c r="N376" s="12"/>
     </row>
     <row r="377" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A377">
@@ -36886,7 +36828,6 @@
         <f t="shared" si="17"/>
         <v>26.143055555556202</v>
       </c>
-      <c r="N377" s="12"/>
     </row>
     <row r="378" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A378">
@@ -36921,7 +36862,7 @@
         <f>VLOOKUP(C378,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>1.5806451612903225</v>
       </c>
-      <c r="N378" s="12">
+      <c r="N378">
         <f>VLOOKUP(C378,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2422.2291666666665</v>
       </c>
@@ -36959,7 +36900,7 @@
         <f>VLOOKUP(C379,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>0.74193548387096775</v>
       </c>
-      <c r="N379" s="12">
+      <c r="N379">
         <f>VLOOKUP(C379,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2383.65625</v>
       </c>
@@ -36997,7 +36938,7 @@
         <f>VLOOKUP(C380,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>0.5</v>
       </c>
-      <c r="N380" s="12">
+      <c r="N380">
         <f>VLOOKUP(C380,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2468.4791666666665</v>
       </c>
@@ -37035,7 +36976,7 @@
         <f>VLOOKUP(C381,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>0.4838709677419355</v>
       </c>
-      <c r="N381" s="12">
+      <c r="N381">
         <f>VLOOKUP(C381,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2510.2395833333335</v>
       </c>
@@ -37069,7 +37010,6 @@
         <f>VLOOKUP(sampling!C382,fe_plate_1!$C$2:$G$300,5,FALSE)</f>
         <v>31.717400000000001</v>
       </c>
-      <c r="N382" s="12"/>
     </row>
     <row r="383" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A383">
@@ -37100,7 +37040,6 @@
         <f>VLOOKUP(sampling!C383,fe_plate_1!$C$2:$G$300,5,FALSE)</f>
         <v>18.103399999999997</v>
       </c>
-      <c r="N383" s="12"/>
     </row>
     <row r="384" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A384">
@@ -37131,7 +37070,6 @@
         <f>VLOOKUP(sampling!C384,fe_plate_1!$C$2:$G$300,5,FALSE)</f>
         <v>37.163000000000011</v>
       </c>
-      <c r="N384" s="12"/>
     </row>
     <row r="385" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A385">
@@ -37162,7 +37100,6 @@
         <f>VLOOKUP(sampling!C385,fe_plate_1!$C$2:$G$300,5,FALSE)</f>
         <v>21.506900000000005</v>
       </c>
-      <c r="N385" s="12"/>
     </row>
     <row r="386" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A386">
@@ -37189,7 +37126,6 @@
         <f t="shared" si="17"/>
         <v>27.180555555554747</v>
       </c>
-      <c r="N386" s="12"/>
     </row>
     <row r="387" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A387">
@@ -37216,7 +37152,6 @@
         <f t="shared" si="17"/>
         <v>27.180555555554747</v>
       </c>
-      <c r="N387" s="12"/>
     </row>
     <row r="388" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A388">
@@ -37243,7 +37178,6 @@
         <f t="shared" ref="G388:G451" si="20" xml:space="preserve"> F388-IF(OR(B388=1,B388=2),$O$2,$O$3)</f>
         <v>27.170833333337214</v>
       </c>
-      <c r="N388" s="12"/>
     </row>
     <row r="389" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A389">
@@ -37270,7 +37204,6 @@
         <f t="shared" si="20"/>
         <v>27.170833333337214</v>
       </c>
-      <c r="N389" s="12"/>
     </row>
     <row r="390" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A390">
@@ -37305,7 +37238,7 @@
         <f>VLOOKUP(C390,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>0</v>
       </c>
-      <c r="N390" s="12">
+      <c r="N390">
         <f>VLOOKUP(C390,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2399.7604166666665</v>
       </c>
@@ -37343,7 +37276,7 @@
         <f>VLOOKUP(C391,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>0</v>
       </c>
-      <c r="N391" s="12">
+      <c r="N391">
         <f>VLOOKUP(C391,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2324.6041666666665</v>
       </c>
@@ -37381,7 +37314,7 @@
         <f>VLOOKUP(C392,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>0</v>
       </c>
-      <c r="N392" s="12">
+      <c r="N392">
         <f>VLOOKUP(C392,new_data!$C$2:$L$221,10,FALSE)/96*1000</f>
         <v>2451.2708333333335</v>
       </c>
@@ -37415,7 +37348,6 @@
         <f>VLOOKUP(C393,new_data!$C$2:$L$221,9,FALSE)/62*1000</f>
         <v>0</v>
       </c>
-      <c r="N393" s="12"/>
     </row>
     <row r="394" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A394">
@@ -37446,7 +37378,6 @@
         <f>VLOOKUP(sampling!C394,fe_plate_1!$C$2:$G$300,5,FALSE)</f>
         <v>11.296400000000002</v>
       </c>
-      <c r="N394" s="12"/>
     </row>
     <row r="395" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A395">
@@ -37477,7 +37408,6 @@
         <f>VLOOKUP(sampling!C395,fe_plate_1!$C$2:$G$300,5,FALSE)</f>
         <v>26.27180000000001</v>
       </c>
-      <c r="N395" s="12"/>
     </row>
     <row r="396" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A396">
@@ -37508,7 +37438,6 @@
         <f>VLOOKUP(sampling!C396,fe_plate_1!$C$2:$G$300,5,FALSE)</f>
         <v>16.061300000000006</v>
       </c>
-      <c r="N396" s="12"/>
     </row>
     <row r="397" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A397">
@@ -37539,7 +37468,6 @@
         <f>VLOOKUP(sampling!C397,fe_plate_1!$C$2:$G$300,5,FALSE)</f>
         <v>19.4648</v>
       </c>
-      <c r="N397" s="12"/>
     </row>
     <row r="398" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A398">
@@ -37566,7 +37494,6 @@
         <f t="shared" si="20"/>
         <v>28.149305555554747</v>
       </c>
-      <c r="N398" s="12"/>
     </row>
     <row r="399" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A399">
@@ -37593,7 +37520,6 @@
         <f t="shared" si="20"/>
         <v>28.149305555554747</v>
       </c>
-      <c r="N399" s="12"/>
     </row>
     <row r="400" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A400">
@@ -37620,9 +37546,8 @@
         <f t="shared" si="20"/>
         <v>28.139583333337214</v>
       </c>
-      <c r="N400" s="12"/>
-    </row>
-    <row r="401" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="401" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A401">
         <v>100</v>
       </c>
@@ -37647,9 +37572,8 @@
         <f t="shared" si="20"/>
         <v>28.139583333337214</v>
       </c>
-      <c r="N401" s="12"/>
-    </row>
-    <row r="402" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="402" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A402">
         <v>101</v>
       </c>
@@ -37674,9 +37598,8 @@
         <f t="shared" si="20"/>
         <v>28.661458333335759</v>
       </c>
-      <c r="N402" s="12"/>
-    </row>
-    <row r="403" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="403" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A403">
         <v>101</v>
       </c>
@@ -37701,9 +37624,8 @@
         <f t="shared" si="20"/>
         <v>28.661458333335759</v>
       </c>
-      <c r="N403" s="12"/>
-    </row>
-    <row r="404" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="404" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A404">
         <v>101</v>
       </c>
@@ -37728,9 +37650,8 @@
         <f t="shared" si="20"/>
         <v>28.651736111118225</v>
       </c>
-      <c r="N404" s="12"/>
-    </row>
-    <row r="405" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="405" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A405">
         <v>101</v>
       </c>
@@ -37755,9 +37676,8 @@
         <f t="shared" si="20"/>
         <v>28.651736111118225</v>
       </c>
-      <c r="N405" s="12"/>
-    </row>
-    <row r="406" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="406" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A406">
         <v>102</v>
       </c>
@@ -37786,9 +37706,8 @@
         <f>VLOOKUP(sampling!C406,fe_plate_1!$C$2:$G$300,5,FALSE)</f>
         <v>35.801600000000008</v>
       </c>
-      <c r="N406" s="12"/>
-    </row>
-    <row r="407" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="407" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A407">
         <v>102</v>
       </c>
@@ -37817,9 +37736,8 @@
         <f>VLOOKUP(sampling!C407,fe_plate_1!$C$2:$G$300,5,FALSE)</f>
         <v>33.078800000000001</v>
       </c>
-      <c r="N407" s="12"/>
-    </row>
-    <row r="408" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="408" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A408">
         <v>102</v>
       </c>
@@ -37848,9 +37766,8 @@
         <f>VLOOKUP(sampling!C408,fe_plate_1!$C$2:$G$300,5,FALSE)</f>
         <v>41.927900000000008</v>
       </c>
-      <c r="N408" s="12"/>
-    </row>
-    <row r="409" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="409" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A409">
         <v>102</v>
       </c>
@@ -37879,9 +37796,8 @@
         <f>VLOOKUP(sampling!C409,fe_plate_1!$C$2:$G$300,5,FALSE)</f>
         <v>19.4648</v>
       </c>
-      <c r="N409" s="12"/>
-    </row>
-    <row r="410" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="410" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A410">
         <v>103</v>
       </c>
@@ -37906,9 +37822,8 @@
         <f t="shared" si="20"/>
         <v>29.223263888889051</v>
       </c>
-      <c r="N410" s="12"/>
-    </row>
-    <row r="411" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="411" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A411">
         <v>103</v>
       </c>
@@ -37933,9 +37848,8 @@
         <f t="shared" si="20"/>
         <v>29.223263888889051</v>
       </c>
-      <c r="N411" s="12"/>
-    </row>
-    <row r="412" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="412" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A412">
         <v>103</v>
       </c>
@@ -37960,9 +37874,8 @@
         <f t="shared" si="20"/>
         <v>29.213541666671517</v>
       </c>
-      <c r="N412" s="12"/>
-    </row>
-    <row r="413" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="413" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A413">
         <v>103</v>
       </c>
@@ -37987,9 +37900,8 @@
         <f t="shared" si="20"/>
         <v>29.213541666671517</v>
       </c>
-      <c r="N413" s="12"/>
-    </row>
-    <row r="414" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="414" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A414">
         <v>104</v>
       </c>
@@ -38014,9 +37926,8 @@
         <f t="shared" si="20"/>
         <v>29.63749999999709</v>
       </c>
-      <c r="N414" s="12"/>
-    </row>
-    <row r="415" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="415" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A415">
         <v>104</v>
       </c>
@@ -38041,9 +37952,8 @@
         <f t="shared" si="20"/>
         <v>29.63749999999709</v>
       </c>
-      <c r="N415" s="12"/>
-    </row>
-    <row r="416" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="416" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A416">
         <v>104</v>
       </c>
@@ -38068,9 +37978,8 @@
         <f t="shared" si="20"/>
         <v>29.627777777779556</v>
       </c>
-      <c r="N416" s="12"/>
-    </row>
-    <row r="417" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="417" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A417">
         <v>104</v>
       </c>
@@ -38095,9 +38004,8 @@
         <f t="shared" si="20"/>
         <v>29.627777777779556</v>
       </c>
-      <c r="N417" s="12"/>
-    </row>
-    <row r="418" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="418" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A418">
         <v>105</v>
       </c>
@@ -38126,9 +38034,8 @@
         <f>VLOOKUP(sampling!C418,fe_plate_1!$C$2:$G$300,5,FALSE)</f>
         <v>30.356000000000005</v>
       </c>
-      <c r="N418" s="12"/>
-    </row>
-    <row r="419" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="419" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A419">
         <v>105</v>
       </c>
@@ -38157,9 +38064,8 @@
         <f>VLOOKUP(sampling!C419,fe_plate_1!$C$2:$G$300,5,FALSE)</f>
         <v>35.801600000000008</v>
       </c>
-      <c r="N419" s="12"/>
-    </row>
-    <row r="420" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="420" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A420">
         <v>105</v>
       </c>
@@ -38188,9 +38094,8 @@
         <f>VLOOKUP(sampling!C420,fe_plate_1!$C$2:$G$300,5,FALSE)</f>
         <v>50.777000000000001</v>
       </c>
-      <c r="N420" s="12"/>
-    </row>
-    <row r="421" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="421" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A421">
         <v>105</v>
       </c>
@@ -38219,9 +38124,8 @@
         <f>VLOOKUP(sampling!C421,fe_plate_1!$C$2:$G$300,5,FALSE)</f>
         <v>22.187600000000007</v>
       </c>
-      <c r="N421" s="12"/>
-    </row>
-    <row r="422" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="422" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A422">
         <v>106</v>
       </c>
@@ -38246,9 +38150,8 @@
         <f t="shared" si="20"/>
         <v>30.214583333327028</v>
       </c>
-      <c r="N422" s="12"/>
-    </row>
-    <row r="423" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="423" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A423">
         <v>106</v>
       </c>
@@ -38273,9 +38176,8 @@
         <f t="shared" si="20"/>
         <v>30.214583333327028</v>
       </c>
-      <c r="N423" s="12"/>
-    </row>
-    <row r="424" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="424" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A424">
         <v>106</v>
       </c>
@@ -38300,9 +38202,8 @@
         <f t="shared" si="20"/>
         <v>30.204861111109494</v>
       </c>
-      <c r="N424" s="12"/>
-    </row>
-    <row r="425" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="425" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A425">
         <v>106</v>
       </c>
@@ -38327,9 +38228,8 @@
         <f t="shared" si="20"/>
         <v>30.204861111109494</v>
       </c>
-      <c r="N425" s="12"/>
-    </row>
-    <row r="426" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="426" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A426">
         <v>107</v>
       </c>
@@ -38354,9 +38254,8 @@
         <f t="shared" si="20"/>
         <v>30.563194444439432</v>
       </c>
-      <c r="N426" s="12"/>
-    </row>
-    <row r="427" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="427" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A427">
         <v>107</v>
       </c>
@@ -38381,9 +38280,8 @@
         <f t="shared" si="20"/>
         <v>30.563194444439432</v>
       </c>
-      <c r="N427" s="12"/>
-    </row>
-    <row r="428" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="428" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A428">
         <v>107</v>
       </c>
@@ -38408,9 +38306,8 @@
         <f t="shared" si="20"/>
         <v>30.553472222221899</v>
       </c>
-      <c r="N428" s="12"/>
-    </row>
-    <row r="429" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="429" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A429">
         <v>107</v>
       </c>
@@ -38435,9 +38332,8 @@
         <f t="shared" si="20"/>
         <v>30.553472222221899</v>
       </c>
-      <c r="N429" s="12"/>
-    </row>
-    <row r="430" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="430" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A430">
         <v>108</v>
       </c>
@@ -38466,9 +38362,8 @@
         <f>VLOOKUP(sampling!C430,fe_plate_1!$C$2:$G$300,5,FALSE)</f>
         <v>32.398099999999999</v>
       </c>
-      <c r="N430" s="12"/>
-    </row>
-    <row r="431" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="431" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A431">
         <v>108</v>
       </c>
@@ -38497,9 +38392,8 @@
         <f>VLOOKUP(sampling!C431,fe_plate_1!$C$2:$G$300,5,FALSE)</f>
         <v>31.0367</v>
       </c>
-      <c r="N431" s="12"/>
-    </row>
-    <row r="432" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="432" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A432">
         <v>108</v>
       </c>
@@ -38528,9 +38422,8 @@
         <f>VLOOKUP(sampling!C432,fe_plate_1!$C$2:$G$300,5,FALSE)</f>
         <v>26.27180000000001</v>
       </c>
-      <c r="N432" s="12"/>
-    </row>
-    <row r="433" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="433" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A433">
         <v>108</v>
       </c>
@@ -38559,9 +38452,8 @@
         <f>VLOOKUP(sampling!C433,fe_plate_1!$C$2:$G$300,5,FALSE)</f>
         <v>21.506900000000005</v>
       </c>
-      <c r="N433" s="12"/>
-    </row>
-    <row r="434" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="434" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A434">
         <v>109</v>
       </c>
@@ -38586,9 +38478,8 @@
         <f t="shared" si="20"/>
         <v>31.189236111109494</v>
       </c>
-      <c r="N434" s="12"/>
-    </row>
-    <row r="435" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="435" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A435">
         <v>109</v>
       </c>
@@ -38613,9 +38504,8 @@
         <f t="shared" si="20"/>
         <v>31.189236111109494</v>
       </c>
-      <c r="N435" s="12"/>
-    </row>
-    <row r="436" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="436" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A436">
         <v>109</v>
       </c>
@@ -38640,9 +38530,8 @@
         <f t="shared" si="20"/>
         <v>31.179513888891961</v>
       </c>
-      <c r="N436" s="12"/>
-    </row>
-    <row r="437" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="437" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A437">
         <v>109</v>
       </c>
@@ -38667,9 +38556,8 @@
         <f t="shared" si="20"/>
         <v>31.179513888891961</v>
       </c>
-      <c r="N437" s="12"/>
-    </row>
-    <row r="438" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="438" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A438">
         <v>110</v>
       </c>
@@ -38698,9 +38586,8 @@
         <f>VLOOKUP(sampling!C438,standard_curve_plate_3!$C$2:$G$404,5,FALSE)</f>
         <v>1.0524360000000001</v>
       </c>
-      <c r="N438" s="12"/>
-    </row>
-    <row r="439" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="439" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A439">
         <v>110</v>
       </c>
@@ -38729,9 +38616,8 @@
         <f>VLOOKUP(sampling!C439,standard_curve_plate_3!$C$2:$G$404,5,FALSE)</f>
         <v>0.4508580000000002</v>
       </c>
-      <c r="N439" s="12"/>
-    </row>
-    <row r="440" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="440" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A440">
         <v>110</v>
       </c>
@@ -38760,9 +38646,8 @@
         <f>VLOOKUP(sampling!C440,standard_curve_plate_3!$C$2:$G$404,5,FALSE)</f>
         <v>-0.28440399999999988</v>
       </c>
-      <c r="N440" s="12"/>
-    </row>
-    <row r="441" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="441" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A441">
         <v>110</v>
       </c>
@@ -38791,9 +38676,8 @@
         <f>VLOOKUP(sampling!C441,standard_curve_plate_3!$C$2:$G$404,5,FALSE)</f>
         <v>-8.3877999999999897E-2</v>
       </c>
-      <c r="N441" s="12"/>
-    </row>
-    <row r="442" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="442" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A442">
         <v>111</v>
       </c>
@@ -38822,9 +38706,8 @@
         <f>VLOOKUP(sampling!C442,fe_plate_1!$C$2:$G$300,5,FALSE)</f>
         <v>31.717400000000001</v>
       </c>
-      <c r="N442" s="12"/>
-    </row>
-    <row r="443" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="443" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A443">
         <v>111</v>
       </c>
@@ -38853,9 +38736,8 @@
         <f>VLOOKUP(sampling!C443,fe_plate_1!$C$2:$G$300,5,FALSE)</f>
         <v>35.120900000000006</v>
       </c>
-      <c r="N443" s="12"/>
-    </row>
-    <row r="444" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="444" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A444">
         <v>111</v>
       </c>
@@ -38884,9 +38766,8 @@
         <f>VLOOKUP(sampling!C444,fe_plate_1!$C$2:$G$300,5,FALSE)</f>
         <v>76.643600000000006</v>
       </c>
-      <c r="N444" s="12"/>
-    </row>
-    <row r="445" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="445" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A445">
         <v>111</v>
       </c>
@@ -38915,9 +38796,8 @@
         <f>VLOOKUP(sampling!C445,fe_plate_1!$C$2:$G$300,5,FALSE)</f>
         <v>23.549000000000003</v>
       </c>
-      <c r="N445" s="12"/>
-    </row>
-    <row r="446" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="446" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A446">
         <v>112</v>
       </c>
@@ -38942,9 +38822,8 @@
         <f t="shared" si="20"/>
         <v>32.230902777773736</v>
       </c>
-      <c r="N446" s="12"/>
-    </row>
-    <row r="447" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="447" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A447">
         <v>112</v>
       </c>
@@ -38969,9 +38848,8 @@
         <f t="shared" si="20"/>
         <v>32.230902777773736</v>
       </c>
-      <c r="N447" s="12"/>
-    </row>
-    <row r="448" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="448" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A448">
         <v>112</v>
       </c>
@@ -38996,9 +38874,8 @@
         <f t="shared" si="20"/>
         <v>32.221180555556202</v>
       </c>
-      <c r="N448" s="12"/>
-    </row>
-    <row r="449" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="449" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A449">
         <v>112</v>
       </c>
@@ -39023,9 +38900,8 @@
         <f t="shared" si="20"/>
         <v>32.221180555556202</v>
       </c>
-      <c r="N449" s="12"/>
-    </row>
-    <row r="450" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="450" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A450">
         <v>113</v>
       </c>
@@ -39054,9 +38930,8 @@
         <f>VLOOKUP(sampling!C450,standard_curve_plate_3!$C$2:$G$404,5,FALSE)</f>
         <v>-0.15071999999999974</v>
       </c>
-      <c r="N450" s="12"/>
-    </row>
-    <row r="451" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="451" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A451">
         <v>113</v>
       </c>
@@ -39085,9 +38960,8 @@
         <f>VLOOKUP(sampling!C451,standard_curve_plate_3!$C$2:$G$404,5,FALSE)</f>
         <v>-0.15071999999999974</v>
       </c>
-      <c r="N451" s="12"/>
-    </row>
-    <row r="452" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="452" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A452">
         <v>113</v>
       </c>
@@ -39116,9 +38990,8 @@
         <f>VLOOKUP(sampling!C452,standard_curve_plate_3!$C$2:$G$404,5,FALSE)</f>
         <v>-0.21756200000000003</v>
       </c>
-      <c r="N452" s="12"/>
-    </row>
-    <row r="453" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="453" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A453">
         <v>113</v>
       </c>
@@ -39147,9 +39020,8 @@
         <f>VLOOKUP(sampling!C453,standard_curve_plate_3!$C$2:$G$404,5,FALSE)</f>
         <v>0.91875200000000001</v>
       </c>
-      <c r="N453" s="12"/>
-    </row>
-    <row r="454" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="454" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A454">
         <v>114</v>
       </c>
@@ -39178,9 +39050,8 @@
         <f>VLOOKUP(sampling!C454,fe_plate_1!$C$2:$G$300,5,FALSE)</f>
         <v>33.078800000000001</v>
       </c>
-      <c r="N454" s="12"/>
-    </row>
-    <row r="455" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="455" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A455">
         <v>114</v>
       </c>
@@ -39209,9 +39080,8 @@
         <f>VLOOKUP(sampling!C455,fe_plate_1!$C$2:$G$300,5,FALSE)</f>
         <v>43.289300000000011</v>
       </c>
-      <c r="N455" s="12"/>
-    </row>
-    <row r="456" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="456" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A456">
         <v>114</v>
       </c>
@@ -39240,9 +39110,8 @@
         <f>VLOOKUP(sampling!C456,fe_plate_1!$C$2:$G$300,5,FALSE)</f>
         <v>30.356000000000005</v>
       </c>
-      <c r="N456" s="12"/>
-    </row>
-    <row r="457" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="457" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A457">
         <v>114</v>
       </c>
@@ -39271,9 +39140,8 @@
         <f>VLOOKUP(sampling!C457,fe_plate_1!$C$2:$G$300,5,FALSE)</f>
         <v>22.187600000000007</v>
       </c>
-      <c r="N457" s="12"/>
-    </row>
-    <row r="458" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="458" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A458">
         <v>115</v>
       </c>
@@ -39298,9 +39166,8 @@
         <f t="shared" si="23"/>
         <v>33.251041666662786</v>
       </c>
-      <c r="N458" s="12"/>
-    </row>
-    <row r="459" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="459" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A459">
         <v>115</v>
       </c>
@@ -39325,9 +39192,8 @@
         <f t="shared" si="23"/>
         <v>33.251041666662786</v>
       </c>
-      <c r="N459" s="12"/>
-    </row>
-    <row r="460" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="460" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A460">
         <v>115</v>
       </c>
@@ -39352,9 +39218,8 @@
         <f t="shared" si="23"/>
         <v>33.241319444445253</v>
       </c>
-      <c r="N460" s="12"/>
-    </row>
-    <row r="461" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="461" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A461">
         <v>115</v>
       </c>
@@ -39379,9 +39244,8 @@
         <f t="shared" si="23"/>
         <v>33.241319444445253</v>
       </c>
-      <c r="N461" s="12"/>
-    </row>
-    <row r="462" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="462" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A462">
         <v>116</v>
       </c>
@@ -39406,9 +39270,8 @@
         <f t="shared" si="23"/>
         <v>34.210763888891961</v>
       </c>
-      <c r="N462" s="12"/>
-    </row>
-    <row r="463" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="463" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A463">
         <v>116</v>
       </c>
@@ -39433,9 +39296,8 @@
         <f t="shared" si="23"/>
         <v>34.210763888891961</v>
       </c>
-      <c r="N463" s="12"/>
-    </row>
-    <row r="464" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="464" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A464">
         <v>116</v>
       </c>
@@ -39460,9 +39322,8 @@
         <f t="shared" si="23"/>
         <v>34.201041666674428</v>
       </c>
-      <c r="N464" s="12"/>
-    </row>
-    <row r="465" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="465" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A465">
         <v>116</v>
       </c>
@@ -39487,7 +39348,6 @@
         <f t="shared" si="23"/>
         <v>34.201041666674428</v>
       </c>
-      <c r="N465" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>